<commit_message>
dummy sd data file updated
</commit_message>
<xml_diff>
--- a/DummyDataSD.xlsx
+++ b/DummyDataSD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\dummyRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CBD8E8-4C70-44CB-BAD3-D7EE4EBB8040}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8DB9EE-BD57-48F5-AA5F-4A6D429EE7F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{53814407-132E-4781-821F-A24DB13BF6DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>sigma</t>
   </si>
@@ -310,39 +310,6 @@
   </si>
   <si>
     <t>AB128</t>
-  </si>
-  <si>
-    <t>AB129</t>
-  </si>
-  <si>
-    <t>AB130</t>
-  </si>
-  <si>
-    <t>AB131</t>
-  </si>
-  <si>
-    <t>AB132</t>
-  </si>
-  <si>
-    <t>AB133</t>
-  </si>
-  <si>
-    <t>AB134</t>
-  </si>
-  <si>
-    <t>AB135</t>
-  </si>
-  <si>
-    <t>AB136</t>
-  </si>
-  <si>
-    <t>AB137</t>
-  </si>
-  <si>
-    <t>AB138</t>
-  </si>
-  <si>
-    <t>AB139</t>
   </si>
 </sst>
 </file>
@@ -806,10 +773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C5F4D2-925C-4D20-9E11-7FE796D1FD56}">
-  <dimension ref="A1:BP101"/>
+  <dimension ref="A1:BP89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B41"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,19 +1225,19 @@
         <v>68</v>
       </c>
       <c r="C4" s="8">
-        <f t="shared" ref="C4:C41" si="0">AVERAGEIF(G4:BO4,"&lt;&gt;0")</f>
+        <f t="shared" ref="C4:C29" si="0">AVERAGEIF(G4:BO4,"&lt;&gt;0")</f>
         <v>8.5399999999999991</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D41" si="1">_xlfn.STDEV.P(G4:BO4)</f>
+        <f t="shared" ref="D4:D29" si="1">_xlfn.STDEV.P(G4:BO4)</f>
         <v>9.8029771322663866</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" ref="E4:E41" si="2">C4+$E$1*D4</f>
+        <f t="shared" ref="E4:E29" si="2">C4+$E$1*D4</f>
         <v>37.948931396799161</v>
       </c>
       <c r="F4" s="10">
-        <f t="shared" ref="F4:F41" si="3">C4-$E$1*D4</f>
+        <f t="shared" ref="F4:F29" si="3">C4-$E$1*D4</f>
         <v>-20.868931396799162</v>
       </c>
       <c r="G4" s="11">
@@ -1456,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="BP4" s="12">
-        <f t="shared" ref="BP4:BP41" si="4">SUM(G4:BO4)</f>
+        <f t="shared" ref="BP4:BP29" si="4">SUM(G4:BO4)</f>
         <v>427</v>
       </c>
     </row>
@@ -5267,19 +5235,19 @@
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
-        <v>263.33333333333331</v>
+        <v>263.11764705882354</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="1"/>
-        <v>511.90310879856457</v>
+        <v>511.96220057072793</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="2"/>
-        <v>1799.042659729027</v>
+        <v>1799.0042487710075</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="3"/>
-        <v>-1272.3759930623605</v>
+        <v>-1272.7689546533602</v>
       </c>
       <c r="G23" s="11">
         <v>0</v>
@@ -5447,7 +5415,7 @@
         <v>107</v>
       </c>
       <c r="BJ23" s="11">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="BK23" s="11">
         <v>36</v>
@@ -5459,14 +5427,14 @@
         <v>24</v>
       </c>
       <c r="BN23" s="11">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BO23" s="11">
         <v>0</v>
       </c>
       <c r="BP23" s="12">
         <f t="shared" si="4"/>
-        <v>13430</v>
+        <v>13419</v>
       </c>
     </row>
     <row r="24" spans="1:68" x14ac:dyDescent="0.25">
@@ -5478,19 +5446,19 @@
       </c>
       <c r="C24" s="8">
         <f t="shared" si="0"/>
-        <v>97.6</v>
+        <v>90.51666666666668</v>
       </c>
       <c r="D24" s="9">
         <f t="shared" si="1"/>
-        <v>200.52292293638357</v>
+        <v>200.51077427906142</v>
       </c>
       <c r="E24" s="9">
         <f t="shared" si="2"/>
-        <v>699.16876880915072</v>
+        <v>692.04898950385086</v>
       </c>
       <c r="F24" s="10">
         <f t="shared" si="3"/>
-        <v>-503.96876880915067</v>
+        <v>-511.01565617051756</v>
       </c>
       <c r="G24" s="11">
         <v>0</v>
@@ -5613,7 +5581,7 @@
         <v>10</v>
       </c>
       <c r="AU24" s="11">
-        <v>8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AV24" s="11">
         <v>0</v>
@@ -5631,7 +5599,7 @@
         <v>0</v>
       </c>
       <c r="BA24" s="11">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="BB24" s="11">
         <v>0</v>
@@ -5658,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="BJ24" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK24" s="11">
         <v>0</v>
@@ -5677,7 +5645,7 @@
       </c>
       <c r="BP24" s="12">
         <f t="shared" si="4"/>
-        <v>2440</v>
+        <v>2443.9500000000003</v>
       </c>
     </row>
     <row r="25" spans="1:68" x14ac:dyDescent="0.25">
@@ -6737,44 +6705,44 @@
     </row>
     <row r="30" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C30" s="8">
-        <f t="shared" si="0"/>
-        <v>12.794871794871796</v>
+        <f t="shared" ref="C30" si="5">AVERAGEIF(G30:BO30,"&lt;&gt;0")</f>
+        <v>8.3414634146341466</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" si="1"/>
-        <v>29.289682733798951</v>
+        <f t="shared" ref="D30" si="6">_xlfn.STDEV.P(G30:BO30)</f>
+        <v>9.7245315762691327</v>
       </c>
       <c r="E30" s="9">
-        <f t="shared" si="2"/>
-        <v>100.66391999626865</v>
+        <f t="shared" ref="E30" si="7">C30+$E$1*D30</f>
+        <v>37.515058143441543</v>
       </c>
       <c r="F30" s="10">
-        <f t="shared" si="3"/>
-        <v>-75.074176406525055</v>
+        <f t="shared" ref="F30" si="8">C30-$E$1*D30</f>
+        <v>-20.832131314173253</v>
       </c>
       <c r="G30" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L30" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="11">
         <v>0</v>
@@ -6783,97 +6751,97 @@
         <v>0</v>
       </c>
       <c r="O30" s="11">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="P30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="11">
         <v>0</v>
       </c>
       <c r="R30" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S30" s="11">
         <v>0</v>
       </c>
       <c r="T30" s="11">
-        <v>229</v>
+        <v>44</v>
       </c>
       <c r="U30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V30" s="11">
         <v>1</v>
       </c>
       <c r="W30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X30" s="11">
         <v>10</v>
       </c>
       <c r="Y30" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z30" s="11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AA30" s="11">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AB30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="11">
+        <v>13</v>
+      </c>
+      <c r="AD30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AE30" s="11">
         <v>3</v>
       </c>
-      <c r="AC30" s="11">
+      <c r="AF30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AG30" s="11">
         <v>6</v>
       </c>
-      <c r="AD30" s="11">
-        <v>3</v>
-      </c>
-      <c r="AE30" s="11">
-        <v>7</v>
-      </c>
-      <c r="AF30" s="11">
+      <c r="AH30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AI30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AJ30" s="11">
+        <v>6</v>
+      </c>
+      <c r="AK30" s="11">
+        <v>11</v>
+      </c>
+      <c r="AL30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AM30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AO30" s="11">
+        <v>9</v>
+      </c>
+      <c r="AP30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR30" s="11">
         <v>10</v>
       </c>
-      <c r="AG30" s="11">
-        <v>3</v>
-      </c>
-      <c r="AH30" s="11">
-        <v>16</v>
-      </c>
-      <c r="AI30" s="11">
-        <v>19</v>
-      </c>
-      <c r="AJ30" s="11">
-        <v>2</v>
-      </c>
-      <c r="AK30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="11">
-        <v>16</v>
-      </c>
-      <c r="AM30" s="11">
-        <v>13</v>
-      </c>
-      <c r="AN30" s="11">
-        <v>4</v>
-      </c>
-      <c r="AO30" s="11">
-        <v>12</v>
-      </c>
-      <c r="AP30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AQ30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AR30" s="11">
-        <v>37</v>
-      </c>
       <c r="AS30" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT30" s="11">
         <v>0</v>
@@ -6882,2410 +6850,122 @@
         <v>0</v>
       </c>
       <c r="AV30" s="11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AW30" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX30" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY30" s="11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AZ30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA30" s="11">
         <v>0</v>
       </c>
       <c r="BB30" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BC30" s="11">
+        <v>0</v>
+      </c>
+      <c r="BD30" s="11">
         <v>11</v>
       </c>
-      <c r="BD30" s="11">
-        <v>20</v>
-      </c>
       <c r="BE30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF30" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BG30" s="11">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BH30" s="11">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="BI30" s="11">
         <v>0</v>
       </c>
       <c r="BJ30" s="11">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="BK30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BL30" s="11">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="BM30" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BN30" s="11">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="BO30" s="11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="BP30" s="12">
-        <f t="shared" si="4"/>
-        <v>499</v>
+        <f t="shared" ref="BP30" si="9">SUM(G30:BO30)</f>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="8">
-        <f t="shared" si="0"/>
-        <v>217.84090909090909</v>
-      </c>
-      <c r="D31" s="9">
-        <f t="shared" si="1"/>
-        <v>542.07955605741529</v>
-      </c>
-      <c r="E31" s="9">
-        <f t="shared" si="2"/>
-        <v>1844.079577263155</v>
-      </c>
-      <c r="F31" s="10">
-        <f t="shared" si="3"/>
-        <v>-1408.397759081337</v>
-      </c>
-      <c r="G31" s="11">
-        <v>0</v>
-      </c>
-      <c r="H31" s="11">
-        <v>0</v>
-      </c>
-      <c r="I31" s="11">
-        <v>0</v>
-      </c>
-      <c r="J31" s="11">
-        <v>0</v>
-      </c>
-      <c r="K31" s="11">
-        <v>0</v>
-      </c>
-      <c r="L31" s="11">
-        <v>0</v>
-      </c>
-      <c r="M31" s="11">
-        <v>0</v>
-      </c>
-      <c r="N31" s="11">
-        <v>0</v>
-      </c>
-      <c r="O31" s="11">
-        <v>0</v>
-      </c>
-      <c r="P31" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="11">
-        <v>0</v>
-      </c>
-      <c r="R31" s="11">
-        <v>0</v>
-      </c>
-      <c r="S31" s="11">
-        <v>0</v>
-      </c>
-      <c r="T31" s="11">
-        <v>0</v>
-      </c>
-      <c r="U31" s="11">
-        <v>0</v>
-      </c>
-      <c r="V31" s="11">
-        <v>0</v>
-      </c>
-      <c r="W31" s="11">
-        <v>0</v>
-      </c>
-      <c r="X31" s="11">
-        <v>3735</v>
-      </c>
-      <c r="Y31" s="11">
-        <v>76</v>
-      </c>
-      <c r="Z31" s="11">
-        <v>58</v>
-      </c>
-      <c r="AA31" s="11">
-        <v>43</v>
-      </c>
-      <c r="AB31" s="11">
-        <v>55</v>
-      </c>
-      <c r="AC31" s="11">
-        <v>79</v>
-      </c>
-      <c r="AD31" s="11">
-        <v>64</v>
-      </c>
-      <c r="AE31" s="11">
-        <v>39</v>
-      </c>
-      <c r="AF31" s="11">
-        <v>90</v>
-      </c>
-      <c r="AG31" s="11">
-        <v>57</v>
-      </c>
-      <c r="AH31" s="11">
-        <v>61</v>
-      </c>
-      <c r="AI31" s="11">
-        <v>78</v>
-      </c>
-      <c r="AJ31" s="11">
-        <v>321</v>
-      </c>
-      <c r="AK31" s="11">
-        <v>55</v>
-      </c>
-      <c r="AL31" s="11">
-        <v>58</v>
-      </c>
-      <c r="AM31" s="11">
-        <v>59</v>
-      </c>
-      <c r="AN31" s="11">
-        <v>65</v>
-      </c>
-      <c r="AO31" s="11">
-        <v>86</v>
-      </c>
-      <c r="AP31" s="11">
-        <v>62</v>
-      </c>
-      <c r="AQ31" s="11">
-        <v>90</v>
-      </c>
-      <c r="AR31" s="11">
-        <v>52</v>
-      </c>
-      <c r="AS31" s="11">
-        <v>80</v>
-      </c>
-      <c r="AT31" s="11">
-        <v>54</v>
-      </c>
-      <c r="AU31" s="11">
-        <v>70</v>
-      </c>
-      <c r="AV31" s="11">
-        <v>958</v>
-      </c>
-      <c r="AW31" s="11">
-        <v>45</v>
-      </c>
-      <c r="AX31" s="11">
-        <v>83</v>
-      </c>
-      <c r="AY31" s="11">
-        <v>53</v>
-      </c>
-      <c r="AZ31" s="11">
-        <v>60</v>
-      </c>
-      <c r="BA31" s="11">
-        <v>49</v>
-      </c>
-      <c r="BB31" s="11">
-        <v>16</v>
-      </c>
-      <c r="BC31" s="11">
-        <v>66</v>
-      </c>
-      <c r="BD31" s="11">
-        <v>80</v>
-      </c>
-      <c r="BE31" s="11">
-        <v>78</v>
-      </c>
-      <c r="BF31" s="11">
-        <v>38</v>
-      </c>
-      <c r="BG31" s="11">
-        <v>85</v>
-      </c>
-      <c r="BH31" s="11">
-        <v>2069</v>
-      </c>
-      <c r="BI31" s="11">
-        <v>42</v>
-      </c>
-      <c r="BJ31" s="11">
-        <v>58</v>
-      </c>
-      <c r="BK31" s="11">
-        <v>50</v>
-      </c>
-      <c r="BL31" s="11">
-        <v>38</v>
-      </c>
-      <c r="BM31" s="11">
-        <v>48</v>
-      </c>
-      <c r="BN31" s="11">
-        <v>163</v>
-      </c>
-      <c r="BO31" s="11">
-        <v>19</v>
-      </c>
-      <c r="BP31" s="12">
-        <f t="shared" si="4"/>
-        <v>9585</v>
-      </c>
+      <c r="C31"/>
     </row>
     <row r="32" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="8">
-        <f t="shared" si="0"/>
-        <v>83.159090909090907</v>
-      </c>
-      <c r="D32" s="9">
-        <f t="shared" si="1"/>
-        <v>232.81340532380895</v>
-      </c>
-      <c r="E32" s="9">
-        <f t="shared" si="2"/>
-        <v>781.5993068805177</v>
-      </c>
-      <c r="F32" s="10">
-        <f t="shared" si="3"/>
-        <v>-615.28112506233595</v>
-      </c>
-      <c r="G32" s="11">
-        <v>0</v>
-      </c>
-      <c r="H32" s="11">
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
-        <v>0</v>
-      </c>
-      <c r="J32" s="11">
-        <v>0</v>
-      </c>
-      <c r="K32" s="11">
-        <v>0</v>
-      </c>
-      <c r="L32" s="11">
-        <v>0</v>
-      </c>
-      <c r="M32" s="11">
-        <v>0</v>
-      </c>
-      <c r="N32" s="11">
-        <v>0</v>
-      </c>
-      <c r="O32" s="11">
-        <v>0</v>
-      </c>
-      <c r="P32" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="11">
-        <v>0</v>
-      </c>
-      <c r="R32" s="11">
-        <v>0</v>
-      </c>
-      <c r="S32" s="11">
-        <v>0</v>
-      </c>
-      <c r="T32" s="11">
-        <v>0</v>
-      </c>
-      <c r="U32" s="11">
-        <v>0</v>
-      </c>
-      <c r="V32" s="11">
-        <v>0</v>
-      </c>
-      <c r="W32" s="11">
-        <v>0</v>
-      </c>
-      <c r="X32" s="11">
-        <v>1839</v>
-      </c>
-      <c r="Y32" s="11">
-        <v>19</v>
-      </c>
-      <c r="Z32" s="11">
-        <v>14</v>
-      </c>
-      <c r="AA32" s="11">
-        <v>11</v>
-      </c>
-      <c r="AB32" s="11">
-        <v>20</v>
-      </c>
-      <c r="AC32" s="11">
-        <v>45</v>
-      </c>
-      <c r="AD32" s="11">
-        <v>33</v>
-      </c>
-      <c r="AE32" s="11">
-        <v>27</v>
-      </c>
-      <c r="AF32" s="11">
-        <v>30</v>
-      </c>
-      <c r="AG32" s="11">
-        <v>11</v>
-      </c>
-      <c r="AH32" s="11">
-        <v>12</v>
-      </c>
-      <c r="AI32" s="11">
-        <v>32</v>
-      </c>
-      <c r="AJ32" s="11">
-        <v>211</v>
-      </c>
-      <c r="AK32" s="11">
-        <v>36</v>
-      </c>
-      <c r="AL32" s="11">
-        <v>18</v>
-      </c>
-      <c r="AM32" s="11">
-        <v>16</v>
-      </c>
-      <c r="AN32" s="11">
-        <v>29</v>
-      </c>
-      <c r="AO32" s="11">
-        <v>43</v>
-      </c>
-      <c r="AP32" s="11">
-        <v>52</v>
-      </c>
-      <c r="AQ32" s="11">
-        <v>37</v>
-      </c>
-      <c r="AR32" s="11">
-        <v>32</v>
-      </c>
-      <c r="AS32" s="11">
-        <v>76</v>
-      </c>
-      <c r="AT32" s="11">
-        <v>124</v>
-      </c>
-      <c r="AU32" s="11">
-        <v>21</v>
-      </c>
-      <c r="AV32" s="11">
-        <v>134</v>
-      </c>
-      <c r="AW32" s="11">
-        <v>22</v>
-      </c>
-      <c r="AX32" s="11">
-        <v>25</v>
-      </c>
-      <c r="AY32" s="11">
-        <v>28</v>
-      </c>
-      <c r="AZ32" s="11">
-        <v>26</v>
-      </c>
-      <c r="BA32" s="11">
-        <v>40</v>
-      </c>
-      <c r="BB32" s="11">
-        <v>54</v>
-      </c>
-      <c r="BC32" s="11">
-        <v>52</v>
-      </c>
-      <c r="BD32" s="11">
-        <v>65</v>
-      </c>
-      <c r="BE32" s="11">
-        <v>38</v>
-      </c>
-      <c r="BF32" s="11">
-        <v>34</v>
-      </c>
-      <c r="BG32" s="11">
-        <v>64</v>
-      </c>
-      <c r="BH32" s="11">
-        <v>137</v>
-      </c>
-      <c r="BI32" s="11">
-        <v>16</v>
-      </c>
-      <c r="BJ32" s="11">
-        <v>32</v>
-      </c>
-      <c r="BK32" s="11">
-        <v>25</v>
-      </c>
-      <c r="BL32" s="11">
-        <v>19</v>
-      </c>
-      <c r="BM32" s="11">
-        <v>17</v>
-      </c>
-      <c r="BN32" s="11">
-        <v>28</v>
-      </c>
-      <c r="BO32" s="11">
-        <v>15</v>
-      </c>
-      <c r="BP32" s="12">
-        <f t="shared" si="4"/>
-        <v>3659</v>
-      </c>
-    </row>
-    <row r="33" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="8">
-        <f t="shared" si="0"/>
-        <v>13.475409836065573</v>
-      </c>
-      <c r="D33" s="9">
-        <f t="shared" si="1"/>
-        <v>8.3088074095949125</v>
-      </c>
-      <c r="E33" s="9">
-        <f t="shared" si="2"/>
-        <v>38.401832064850311</v>
-      </c>
-      <c r="F33" s="10">
-        <f t="shared" si="3"/>
-        <v>-11.451012392719164</v>
-      </c>
-      <c r="G33" s="11">
-        <v>14</v>
-      </c>
-      <c r="H33" s="11">
-        <v>5</v>
-      </c>
-      <c r="I33" s="11">
-        <v>25</v>
-      </c>
-      <c r="J33" s="11">
-        <v>9</v>
-      </c>
-      <c r="K33" s="11">
-        <v>2</v>
-      </c>
-      <c r="L33" s="11">
-        <v>19</v>
-      </c>
-      <c r="M33" s="11">
-        <v>13</v>
-      </c>
-      <c r="N33" s="11">
-        <v>12</v>
-      </c>
-      <c r="O33" s="11">
-        <v>14</v>
-      </c>
-      <c r="P33" s="11">
-        <v>8</v>
-      </c>
-      <c r="Q33" s="11">
-        <v>11</v>
-      </c>
-      <c r="R33" s="11">
-        <v>15</v>
-      </c>
-      <c r="S33" s="11">
-        <v>10</v>
-      </c>
-      <c r="T33" s="11">
-        <v>12</v>
-      </c>
-      <c r="U33" s="11">
-        <v>24</v>
-      </c>
-      <c r="V33" s="11">
-        <v>16</v>
-      </c>
-      <c r="W33" s="11">
-        <v>13</v>
-      </c>
-      <c r="X33" s="11">
-        <v>18</v>
-      </c>
-      <c r="Y33" s="11">
-        <v>11</v>
-      </c>
-      <c r="Z33" s="11">
-        <v>8</v>
-      </c>
-      <c r="AA33" s="11">
-        <v>2</v>
-      </c>
-      <c r="AB33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AC33" s="11">
-        <v>17</v>
-      </c>
-      <c r="AD33" s="11">
-        <v>14</v>
-      </c>
-      <c r="AE33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AF33" s="11">
-        <v>9</v>
-      </c>
-      <c r="AG33" s="11">
-        <v>40</v>
-      </c>
-      <c r="AH33" s="11">
-        <v>12</v>
-      </c>
-      <c r="AI33" s="11">
-        <v>13</v>
-      </c>
-      <c r="AJ33" s="11">
-        <v>13</v>
-      </c>
-      <c r="AK33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AL33" s="11">
-        <v>20</v>
-      </c>
-      <c r="AM33" s="11">
-        <v>10</v>
-      </c>
-      <c r="AN33" s="11">
-        <v>8</v>
-      </c>
-      <c r="AO33" s="11">
-        <v>19</v>
-      </c>
-      <c r="AP33" s="11">
-        <v>11</v>
-      </c>
-      <c r="AQ33" s="11">
-        <v>13</v>
-      </c>
-      <c r="AR33" s="11">
-        <v>19</v>
-      </c>
-      <c r="AS33" s="11">
-        <v>6</v>
-      </c>
-      <c r="AT33" s="11">
-        <v>16</v>
-      </c>
-      <c r="AU33" s="11">
-        <v>9</v>
-      </c>
-      <c r="AV33" s="11">
-        <v>29</v>
-      </c>
-      <c r="AW33" s="11">
-        <v>15</v>
-      </c>
-      <c r="AX33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AY33" s="11">
-        <v>6</v>
-      </c>
-      <c r="AZ33" s="11">
-        <v>3</v>
-      </c>
-      <c r="BA33" s="11">
-        <v>14</v>
-      </c>
-      <c r="BB33" s="11">
-        <v>17</v>
-      </c>
-      <c r="BC33" s="11">
-        <v>20</v>
-      </c>
-      <c r="BD33" s="11">
-        <v>12</v>
-      </c>
-      <c r="BE33" s="11">
-        <v>7</v>
-      </c>
-      <c r="BF33" s="11">
-        <v>9</v>
-      </c>
-      <c r="BG33" s="11">
-        <v>9</v>
-      </c>
-      <c r="BH33" s="11">
-        <v>21</v>
-      </c>
-      <c r="BI33" s="11">
-        <v>4</v>
-      </c>
-      <c r="BJ33" s="11">
-        <v>2</v>
-      </c>
-      <c r="BK33" s="11">
-        <v>21</v>
-      </c>
-      <c r="BL33" s="11">
-        <v>24</v>
-      </c>
-      <c r="BM33" s="11">
-        <v>22</v>
-      </c>
-      <c r="BN33" s="11">
-        <v>47</v>
-      </c>
-      <c r="BO33" s="11">
-        <v>10</v>
-      </c>
-      <c r="BP33" s="12">
-        <f t="shared" si="4"/>
-        <v>822</v>
-      </c>
-    </row>
-    <row r="34" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>32</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" s="8">
-        <f t="shared" si="0"/>
-        <v>18.53125</v>
-      </c>
-      <c r="D34" s="9">
-        <f t="shared" si="1"/>
-        <v>48.000044790805944</v>
-      </c>
-      <c r="E34" s="9">
-        <f t="shared" si="2"/>
-        <v>162.53138437241785</v>
-      </c>
-      <c r="F34" s="10">
-        <f t="shared" si="3"/>
-        <v>-125.46888437241785</v>
-      </c>
-      <c r="G34" s="11">
-        <v>0</v>
-      </c>
-      <c r="H34" s="11">
-        <v>0</v>
-      </c>
-      <c r="I34" s="11">
-        <v>0</v>
-      </c>
-      <c r="J34" s="11">
-        <v>0</v>
-      </c>
-      <c r="K34" s="11">
-        <v>0</v>
-      </c>
-      <c r="L34" s="11">
-        <v>0</v>
-      </c>
-      <c r="M34" s="11">
-        <v>0</v>
-      </c>
-      <c r="N34" s="11">
-        <v>0</v>
-      </c>
-      <c r="O34" s="11">
-        <v>0</v>
-      </c>
-      <c r="P34" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="11">
-        <v>0</v>
-      </c>
-      <c r="R34" s="11">
-        <v>0</v>
-      </c>
-      <c r="S34" s="11">
-        <v>0</v>
-      </c>
-      <c r="T34" s="11">
-        <v>0</v>
-      </c>
-      <c r="U34" s="11">
-        <v>0</v>
-      </c>
-      <c r="V34" s="11">
-        <v>0</v>
-      </c>
-      <c r="W34" s="11">
-        <v>0</v>
-      </c>
-      <c r="X34" s="11">
-        <v>379</v>
-      </c>
-      <c r="Y34" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="11">
-        <v>4</v>
-      </c>
-      <c r="AC34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="11">
-        <v>4</v>
-      </c>
-      <c r="AE34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="11">
-        <v>8</v>
-      </c>
-      <c r="AG34" s="11">
-        <v>6</v>
-      </c>
-      <c r="AH34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AI34" s="11">
-        <v>11</v>
-      </c>
-      <c r="AJ34" s="11">
-        <v>19</v>
-      </c>
-      <c r="AK34" s="11">
-        <v>1</v>
-      </c>
-      <c r="AL34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AM34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AN34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AO34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AP34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AQ34" s="11">
-        <v>9</v>
-      </c>
-      <c r="AR34" s="11">
-        <v>9</v>
-      </c>
-      <c r="AS34" s="11">
-        <v>22</v>
-      </c>
-      <c r="AT34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AU34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AV34" s="11">
-        <v>21</v>
-      </c>
-      <c r="AW34" s="11">
-        <v>3</v>
-      </c>
-      <c r="AX34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AY34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ34" s="11">
-        <v>2</v>
-      </c>
-      <c r="BA34" s="11">
-        <v>5</v>
-      </c>
-      <c r="BB34" s="11">
-        <v>3</v>
-      </c>
-      <c r="BC34" s="11">
-        <v>1</v>
-      </c>
-      <c r="BD34" s="11">
-        <v>8</v>
-      </c>
-      <c r="BE34" s="11">
-        <v>6</v>
-      </c>
-      <c r="BF34" s="11">
-        <v>1</v>
-      </c>
-      <c r="BG34" s="11">
-        <v>0</v>
-      </c>
-      <c r="BH34" s="11">
-        <v>20</v>
-      </c>
-      <c r="BI34" s="11">
-        <v>3</v>
-      </c>
-      <c r="BJ34" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK34" s="11">
-        <v>9</v>
-      </c>
-      <c r="BL34" s="11">
-        <v>4</v>
-      </c>
-      <c r="BM34" s="11">
-        <v>1</v>
-      </c>
-      <c r="BN34" s="11">
-        <v>11</v>
-      </c>
-      <c r="BO34" s="11">
-        <v>13</v>
-      </c>
-      <c r="BP34" s="12">
-        <f t="shared" si="4"/>
-        <v>593</v>
-      </c>
-    </row>
-    <row r="35" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>33</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="8">
-        <f t="shared" si="0"/>
-        <v>242.88888888888889</v>
-      </c>
-      <c r="D35" s="9">
-        <f t="shared" si="1"/>
-        <v>415.81600144444019</v>
-      </c>
-      <c r="E35" s="9">
-        <f t="shared" si="2"/>
-        <v>1490.3368932222095</v>
-      </c>
-      <c r="F35" s="10">
-        <f t="shared" si="3"/>
-        <v>-1004.5591154444317</v>
-      </c>
-      <c r="G35" s="11">
-        <v>0</v>
-      </c>
-      <c r="H35" s="11">
-        <v>0</v>
-      </c>
-      <c r="I35" s="11">
-        <v>0</v>
-      </c>
-      <c r="J35" s="11">
-        <v>0</v>
-      </c>
-      <c r="K35" s="11">
-        <v>0</v>
-      </c>
-      <c r="L35" s="11">
-        <v>0</v>
-      </c>
-      <c r="M35" s="11">
-        <v>0</v>
-      </c>
-      <c r="N35" s="11">
-        <v>0</v>
-      </c>
-      <c r="O35" s="11">
-        <v>0</v>
-      </c>
-      <c r="P35" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="11">
-        <v>0</v>
-      </c>
-      <c r="R35" s="11">
-        <v>0</v>
-      </c>
-      <c r="S35" s="11">
-        <v>0</v>
-      </c>
-      <c r="T35" s="11">
-        <v>0</v>
-      </c>
-      <c r="U35" s="11">
-        <v>0</v>
-      </c>
-      <c r="V35" s="11">
-        <v>0</v>
-      </c>
-      <c r="W35" s="11">
-        <v>0</v>
-      </c>
-      <c r="X35" s="11">
-        <v>1581</v>
-      </c>
-      <c r="Y35" s="11">
-        <v>29</v>
-      </c>
-      <c r="Z35" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA35" s="11">
-        <v>22</v>
-      </c>
-      <c r="AB35" s="11">
-        <v>11</v>
-      </c>
-      <c r="AC35" s="11">
-        <v>21</v>
-      </c>
-      <c r="AD35" s="11">
-        <v>48</v>
-      </c>
-      <c r="AE35" s="11">
-        <v>29</v>
-      </c>
-      <c r="AF35" s="11">
-        <v>25</v>
-      </c>
-      <c r="AG35" s="11">
-        <v>10</v>
-      </c>
-      <c r="AH35" s="11">
-        <v>23</v>
-      </c>
-      <c r="AI35" s="11">
-        <v>8</v>
-      </c>
-      <c r="AJ35" s="11">
-        <v>1680</v>
-      </c>
-      <c r="AK35" s="11">
-        <v>30</v>
-      </c>
-      <c r="AL35" s="11">
-        <v>76</v>
-      </c>
-      <c r="AM35" s="11">
-        <v>6</v>
-      </c>
-      <c r="AN35" s="11">
-        <v>35</v>
-      </c>
-      <c r="AO35" s="11">
-        <v>30</v>
-      </c>
-      <c r="AP35" s="11">
-        <v>27</v>
-      </c>
-      <c r="AQ35" s="11">
-        <v>74</v>
-      </c>
-      <c r="AR35" s="11">
-        <v>37</v>
-      </c>
-      <c r="AS35" s="11">
-        <v>30</v>
-      </c>
-      <c r="AT35" s="11">
-        <v>14</v>
-      </c>
-      <c r="AU35" s="11">
-        <v>18</v>
-      </c>
-      <c r="AV35" s="11">
-        <v>1766</v>
-      </c>
-      <c r="AW35" s="11">
-        <v>53</v>
-      </c>
-      <c r="AX35" s="11">
-        <v>22</v>
-      </c>
-      <c r="AY35" s="11">
-        <v>53</v>
-      </c>
-      <c r="AZ35" s="11">
-        <v>57</v>
-      </c>
-      <c r="BA35" s="11">
-        <v>61</v>
-      </c>
-      <c r="BB35" s="11">
-        <v>1645</v>
-      </c>
-      <c r="BC35" s="11">
-        <v>124</v>
-      </c>
-      <c r="BD35" s="11">
-        <v>107</v>
-      </c>
-      <c r="BE35" s="11">
-        <v>93</v>
-      </c>
-      <c r="BF35" s="11">
-        <v>104</v>
-      </c>
-      <c r="BG35" s="11">
-        <v>41</v>
-      </c>
-      <c r="BH35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BI35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BJ35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BL35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BM35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BN35" s="11">
-        <v>754</v>
-      </c>
-      <c r="BO35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP35" s="12">
-        <f t="shared" si="4"/>
-        <v>8744</v>
-      </c>
-    </row>
-    <row r="36" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>34</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="8">
-        <f t="shared" si="0"/>
-        <v>471.33333333333331</v>
-      </c>
-      <c r="D36" s="9">
-        <f t="shared" si="1"/>
-        <v>919.06327322340621</v>
-      </c>
-      <c r="E36" s="9">
-        <f t="shared" si="2"/>
-        <v>3228.5231530035521</v>
-      </c>
-      <c r="F36" s="10">
-        <f t="shared" si="3"/>
-        <v>-2285.8564863368852</v>
-      </c>
-      <c r="G36" s="11">
-        <v>111</v>
-      </c>
-      <c r="H36" s="11">
-        <v>191</v>
-      </c>
-      <c r="I36" s="11">
-        <v>182</v>
-      </c>
-      <c r="J36" s="11">
-        <v>123</v>
-      </c>
-      <c r="K36" s="11">
-        <v>185</v>
-      </c>
-      <c r="L36" s="11">
-        <v>3544</v>
-      </c>
-      <c r="M36" s="11">
-        <v>148</v>
-      </c>
-      <c r="N36" s="11">
-        <v>215</v>
-      </c>
-      <c r="O36" s="11">
-        <v>124</v>
-      </c>
-      <c r="P36" s="11">
-        <v>78</v>
-      </c>
-      <c r="Q36" s="11">
-        <v>91</v>
-      </c>
-      <c r="R36" s="11">
-        <v>109</v>
-      </c>
-      <c r="S36" s="11">
-        <v>159</v>
-      </c>
-      <c r="T36" s="11">
-        <v>125</v>
-      </c>
-      <c r="U36" s="11">
-        <v>56</v>
-      </c>
-      <c r="V36" s="11">
-        <v>180</v>
-      </c>
-      <c r="W36" s="11">
-        <v>424</v>
-      </c>
-      <c r="X36" s="11">
-        <v>3030</v>
-      </c>
-      <c r="Y36" s="11">
-        <v>280</v>
-      </c>
-      <c r="Z36" s="11">
-        <v>137</v>
-      </c>
-      <c r="AA36" s="11">
-        <v>141</v>
-      </c>
-      <c r="AB36" s="11">
-        <v>143</v>
-      </c>
-      <c r="AC36" s="11">
-        <v>73</v>
-      </c>
-      <c r="AD36" s="11">
-        <v>172</v>
-      </c>
-      <c r="AE36" s="11">
-        <v>161</v>
-      </c>
-      <c r="AF36" s="11">
-        <v>206</v>
-      </c>
-      <c r="AG36" s="11">
-        <v>528</v>
-      </c>
-      <c r="AH36" s="11">
-        <v>104</v>
-      </c>
-      <c r="AI36" s="11">
-        <v>141</v>
-      </c>
-      <c r="AJ36" s="11">
-        <v>2896</v>
-      </c>
-      <c r="AK36" s="11">
-        <v>207</v>
-      </c>
-      <c r="AL36" s="11">
-        <v>69</v>
-      </c>
-      <c r="AM36" s="11">
-        <v>161</v>
-      </c>
-      <c r="AN36" s="11">
-        <v>180</v>
-      </c>
-      <c r="AO36" s="11">
-        <v>114</v>
-      </c>
-      <c r="AP36" s="11">
-        <v>124</v>
-      </c>
-      <c r="AQ36" s="11">
-        <v>118</v>
-      </c>
-      <c r="AR36" s="11">
-        <v>164</v>
-      </c>
-      <c r="AS36" s="11">
-        <v>127</v>
-      </c>
-      <c r="AT36" s="11">
-        <v>142</v>
-      </c>
-      <c r="AU36" s="11">
-        <v>106</v>
-      </c>
-      <c r="AV36" s="11">
-        <v>5015</v>
-      </c>
-      <c r="AW36" s="11">
-        <v>299</v>
-      </c>
-      <c r="AX36" s="11">
-        <v>163</v>
-      </c>
-      <c r="AY36" s="11">
-        <v>225</v>
-      </c>
-      <c r="AZ36" s="11">
-        <v>122</v>
-      </c>
-      <c r="BA36" s="11">
-        <v>428</v>
-      </c>
-      <c r="BB36" s="11">
-        <v>279</v>
-      </c>
-      <c r="BC36" s="11">
-        <v>212</v>
-      </c>
-      <c r="BD36" s="11">
-        <v>300</v>
-      </c>
-      <c r="BE36" s="11">
-        <v>278</v>
-      </c>
-      <c r="BF36" s="11">
-        <v>189</v>
-      </c>
-      <c r="BG36" s="11">
-        <v>164</v>
-      </c>
-      <c r="BH36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BI36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BJ36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BL36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BM36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BN36" s="11">
-        <v>2209</v>
-      </c>
-      <c r="BO36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP36" s="12">
-        <f t="shared" si="4"/>
-        <v>25452</v>
-      </c>
-    </row>
-    <row r="37" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>35</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="8">
-        <f t="shared" si="0"/>
-        <v>1406</v>
-      </c>
-      <c r="D37" s="9">
-        <f t="shared" si="1"/>
-        <v>869.45953922655644</v>
-      </c>
-      <c r="E37" s="9">
-        <f t="shared" si="2"/>
-        <v>4014.3786176796693</v>
-      </c>
-      <c r="F37" s="10">
-        <f t="shared" si="3"/>
-        <v>-1202.3786176796693</v>
-      </c>
-      <c r="G37" s="11">
-        <v>0</v>
-      </c>
-      <c r="H37" s="11">
-        <v>0</v>
-      </c>
-      <c r="I37" s="11">
-        <v>0</v>
-      </c>
-      <c r="J37" s="11">
-        <v>0</v>
-      </c>
-      <c r="K37" s="11">
-        <v>0</v>
-      </c>
-      <c r="L37" s="11">
-        <v>0</v>
-      </c>
-      <c r="M37" s="11">
-        <v>0</v>
-      </c>
-      <c r="N37" s="11">
-        <v>0</v>
-      </c>
-      <c r="O37" s="11">
-        <v>0</v>
-      </c>
-      <c r="P37" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="11">
-        <v>0</v>
-      </c>
-      <c r="R37" s="11">
-        <v>0</v>
-      </c>
-      <c r="S37" s="11">
-        <v>0</v>
-      </c>
-      <c r="T37" s="11">
-        <v>0</v>
-      </c>
-      <c r="U37" s="11">
-        <v>0</v>
-      </c>
-      <c r="V37" s="11">
-        <v>0</v>
-      </c>
-      <c r="W37" s="11">
-        <v>0</v>
-      </c>
-      <c r="X37" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AG37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AJ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AK37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AM37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AN37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AO37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AP37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AQ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AR37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AS37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AT37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AU37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AV37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AW37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AX37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AY37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BA37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BB37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BC37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BD37" s="11">
-        <v>169</v>
-      </c>
-      <c r="BE37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BF37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BG37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BH37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BI37" s="11">
-        <v>3</v>
-      </c>
-      <c r="BJ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK37" s="11">
-        <v>7</v>
-      </c>
-      <c r="BL37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BM37" s="11">
-        <v>3</v>
-      </c>
-      <c r="BN37" s="11">
-        <v>6848</v>
-      </c>
-      <c r="BO37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP37" s="12">
-        <f t="shared" si="4"/>
-        <v>7030</v>
-      </c>
-    </row>
-    <row r="38" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>36</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" s="8">
-        <f t="shared" si="0"/>
-        <v>275.29090909090911</v>
-      </c>
-      <c r="D38" s="9">
-        <f t="shared" si="1"/>
-        <v>639.52708231030465</v>
-      </c>
-      <c r="E38" s="9">
-        <f t="shared" si="2"/>
-        <v>2193.8721560218232</v>
-      </c>
-      <c r="F38" s="10">
-        <f t="shared" si="3"/>
-        <v>-1643.2903378400049</v>
-      </c>
-      <c r="G38" s="11">
-        <v>0</v>
-      </c>
-      <c r="H38" s="11">
-        <v>0</v>
-      </c>
-      <c r="I38" s="11">
-        <v>0</v>
-      </c>
-      <c r="J38" s="11">
-        <v>0</v>
-      </c>
-      <c r="K38" s="11">
-        <v>0</v>
-      </c>
-      <c r="L38" s="11">
-        <v>1885</v>
-      </c>
-      <c r="M38" s="11">
-        <v>26</v>
-      </c>
-      <c r="N38" s="11">
-        <v>46</v>
-      </c>
-      <c r="O38" s="11">
-        <v>47</v>
-      </c>
-      <c r="P38" s="11">
-        <v>38</v>
-      </c>
-      <c r="Q38" s="11">
-        <v>41</v>
-      </c>
-      <c r="R38" s="11">
-        <v>60</v>
-      </c>
-      <c r="S38" s="11">
-        <v>74</v>
-      </c>
-      <c r="T38" s="11">
-        <v>40</v>
-      </c>
-      <c r="U38" s="11">
-        <v>49</v>
-      </c>
-      <c r="V38" s="11">
-        <v>75</v>
-      </c>
-      <c r="W38" s="11">
-        <v>33</v>
-      </c>
-      <c r="X38" s="11">
-        <v>2092</v>
-      </c>
-      <c r="Y38" s="11">
-        <v>36</v>
-      </c>
-      <c r="Z38" s="11">
-        <v>37</v>
-      </c>
-      <c r="AA38" s="11">
-        <v>46</v>
-      </c>
-      <c r="AB38" s="11">
-        <v>89</v>
-      </c>
-      <c r="AC38" s="11">
-        <v>35</v>
-      </c>
-      <c r="AD38" s="11">
-        <v>62</v>
-      </c>
-      <c r="AE38" s="11">
-        <v>35</v>
-      </c>
-      <c r="AF38" s="11">
-        <v>66</v>
-      </c>
-      <c r="AG38" s="11">
-        <v>39</v>
-      </c>
-      <c r="AH38" s="11">
-        <v>40</v>
-      </c>
-      <c r="AI38" s="11">
-        <v>25</v>
-      </c>
-      <c r="AJ38" s="11">
-        <v>1855</v>
-      </c>
-      <c r="AK38" s="11">
-        <v>15</v>
-      </c>
-      <c r="AL38" s="11">
-        <v>52</v>
-      </c>
-      <c r="AM38" s="11">
-        <v>49</v>
-      </c>
-      <c r="AN38" s="11">
-        <v>27</v>
-      </c>
-      <c r="AO38" s="11">
-        <v>66</v>
-      </c>
-      <c r="AP38" s="11">
-        <v>35</v>
-      </c>
-      <c r="AQ38" s="11">
-        <v>54</v>
-      </c>
-      <c r="AR38" s="11">
-        <v>37</v>
-      </c>
-      <c r="AS38" s="11">
-        <v>59</v>
-      </c>
-      <c r="AT38" s="11">
-        <v>52</v>
-      </c>
-      <c r="AU38" s="11">
-        <v>37</v>
-      </c>
-      <c r="AV38" s="11">
-        <v>2139</v>
-      </c>
-      <c r="AW38" s="11">
-        <v>41</v>
-      </c>
-      <c r="AX38" s="11">
-        <v>40</v>
-      </c>
-      <c r="AY38" s="11">
-        <v>33</v>
-      </c>
-      <c r="AZ38" s="11">
-        <v>38</v>
-      </c>
-      <c r="BA38" s="11">
-        <v>35</v>
-      </c>
-      <c r="BB38" s="11">
-        <v>39</v>
-      </c>
-      <c r="BC38" s="11">
-        <v>2995</v>
-      </c>
-      <c r="BD38" s="11">
-        <v>142</v>
-      </c>
-      <c r="BE38" s="11">
-        <v>42</v>
-      </c>
-      <c r="BF38" s="11">
-        <v>49</v>
-      </c>
-      <c r="BG38" s="11">
-        <v>14</v>
-      </c>
-      <c r="BH38" s="11">
-        <v>1914</v>
-      </c>
-      <c r="BI38" s="11">
-        <v>61</v>
-      </c>
-      <c r="BJ38" s="11">
-        <v>44</v>
-      </c>
-      <c r="BK38" s="11">
-        <v>22</v>
-      </c>
-      <c r="BL38" s="11">
-        <v>23</v>
-      </c>
-      <c r="BM38" s="11">
-        <v>23</v>
-      </c>
-      <c r="BN38" s="11">
-        <v>93</v>
-      </c>
-      <c r="BO38" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP38" s="12">
-        <f t="shared" si="4"/>
-        <v>15141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
-        <v>37</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="8">
-        <f t="shared" si="0"/>
-        <v>259.27272727272725</v>
-      </c>
-      <c r="D39" s="9">
-        <f t="shared" si="1"/>
-        <v>675.5810223931627</v>
-      </c>
-      <c r="E39" s="9">
-        <f t="shared" si="2"/>
-        <v>2286.0157944522152</v>
-      </c>
-      <c r="F39" s="10">
-        <f t="shared" si="3"/>
-        <v>-1767.470339906761</v>
-      </c>
-      <c r="G39" s="11">
-        <v>0</v>
-      </c>
-      <c r="H39" s="11">
-        <v>0</v>
-      </c>
-      <c r="I39" s="11">
-        <v>0</v>
-      </c>
-      <c r="J39" s="11">
-        <v>0</v>
-      </c>
-      <c r="K39" s="11">
-        <v>0</v>
-      </c>
-      <c r="L39" s="11">
-        <v>1856</v>
-      </c>
-      <c r="M39" s="11">
-        <v>25</v>
-      </c>
-      <c r="N39" s="11">
-        <v>15</v>
-      </c>
-      <c r="O39" s="11">
-        <v>19</v>
-      </c>
-      <c r="P39" s="11">
-        <v>30</v>
-      </c>
-      <c r="Q39" s="11">
-        <v>61</v>
-      </c>
-      <c r="R39" s="11">
-        <v>28</v>
-      </c>
-      <c r="S39" s="11">
-        <v>38</v>
-      </c>
-      <c r="T39" s="11">
-        <v>113</v>
-      </c>
-      <c r="U39" s="11">
-        <v>42</v>
-      </c>
-      <c r="V39" s="11">
-        <v>29</v>
-      </c>
-      <c r="W39" s="11">
-        <v>11</v>
-      </c>
-      <c r="X39" s="11">
-        <v>3756</v>
-      </c>
-      <c r="Y39" s="11">
-        <v>94</v>
-      </c>
-      <c r="Z39" s="11">
-        <v>41</v>
-      </c>
-      <c r="AA39" s="11">
-        <v>50</v>
-      </c>
-      <c r="AB39" s="11">
-        <v>30</v>
-      </c>
-      <c r="AC39" s="11">
-        <v>2004</v>
-      </c>
-      <c r="AD39" s="11">
-        <v>31</v>
-      </c>
-      <c r="AE39" s="11">
-        <v>85</v>
-      </c>
-      <c r="AF39" s="11">
-        <v>128</v>
-      </c>
-      <c r="AG39" s="11">
-        <v>2013</v>
-      </c>
-      <c r="AH39" s="11">
-        <v>12</v>
-      </c>
-      <c r="AI39" s="11">
-        <v>30</v>
-      </c>
-      <c r="AJ39" s="11">
-        <v>2318</v>
-      </c>
-      <c r="AK39" s="11">
-        <v>26</v>
-      </c>
-      <c r="AL39" s="11">
-        <v>14</v>
-      </c>
-      <c r="AM39" s="11">
-        <v>36</v>
-      </c>
-      <c r="AN39" s="11">
-        <v>27</v>
-      </c>
-      <c r="AO39" s="11">
-        <v>12</v>
-      </c>
-      <c r="AP39" s="11">
-        <v>44</v>
-      </c>
-      <c r="AQ39" s="11">
-        <v>21</v>
-      </c>
-      <c r="AR39" s="11">
-        <v>44</v>
-      </c>
-      <c r="AS39" s="11">
-        <v>52</v>
-      </c>
-      <c r="AT39" s="11">
-        <v>40</v>
-      </c>
-      <c r="AU39" s="11">
-        <v>99</v>
-      </c>
-      <c r="AV39" s="11">
-        <v>157</v>
-      </c>
-      <c r="AW39" s="11">
-        <v>28</v>
-      </c>
-      <c r="AX39" s="11">
-        <v>36</v>
-      </c>
-      <c r="AY39" s="11">
-        <v>19</v>
-      </c>
-      <c r="AZ39" s="11">
-        <v>29</v>
-      </c>
-      <c r="BA39" s="11">
-        <v>41</v>
-      </c>
-      <c r="BB39" s="11">
-        <v>212</v>
-      </c>
-      <c r="BC39" s="11">
-        <v>50</v>
-      </c>
-      <c r="BD39" s="11">
-        <v>44</v>
-      </c>
-      <c r="BE39" s="11">
-        <v>25</v>
-      </c>
-      <c r="BF39" s="11">
-        <v>37</v>
-      </c>
-      <c r="BG39" s="11">
-        <v>52</v>
-      </c>
-      <c r="BH39" s="11">
-        <v>57</v>
-      </c>
-      <c r="BI39" s="11">
-        <v>66</v>
-      </c>
-      <c r="BJ39" s="11">
-        <v>24</v>
-      </c>
-      <c r="BK39" s="11">
-        <v>20</v>
-      </c>
-      <c r="BL39" s="11">
-        <v>9</v>
-      </c>
-      <c r="BM39" s="11">
-        <v>19</v>
-      </c>
-      <c r="BN39" s="11">
-        <v>61</v>
-      </c>
-      <c r="BO39" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP39" s="12">
-        <f t="shared" si="4"/>
-        <v>14260</v>
-      </c>
-    </row>
-    <row r="40" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
-        <v>38</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="8">
-        <f t="shared" si="0"/>
-        <v>9.258064516129032</v>
-      </c>
-      <c r="D40" s="9">
-        <f t="shared" si="1"/>
-        <v>18.239161850076371</v>
-      </c>
-      <c r="E40" s="9">
-        <f t="shared" si="2"/>
-        <v>63.975550066358146</v>
-      </c>
-      <c r="F40" s="10">
-        <f t="shared" si="3"/>
-        <v>-45.459421034100082</v>
-      </c>
-      <c r="G40" s="11">
-        <v>0</v>
-      </c>
-      <c r="H40" s="11">
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
-        <v>0</v>
-      </c>
-      <c r="J40" s="11">
-        <v>0</v>
-      </c>
-      <c r="K40" s="11">
-        <v>0</v>
-      </c>
-      <c r="L40" s="11">
-        <v>0</v>
-      </c>
-      <c r="M40" s="11">
-        <v>0</v>
-      </c>
-      <c r="N40" s="11">
-        <v>0</v>
-      </c>
-      <c r="O40" s="11">
-        <v>0</v>
-      </c>
-      <c r="P40" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="11">
-        <v>0</v>
-      </c>
-      <c r="R40" s="11">
-        <v>0</v>
-      </c>
-      <c r="S40" s="11">
-        <v>0</v>
-      </c>
-      <c r="T40" s="11">
-        <v>0</v>
-      </c>
-      <c r="U40" s="11">
-        <v>0</v>
-      </c>
-      <c r="V40" s="11">
-        <v>0</v>
-      </c>
-      <c r="W40" s="11">
-        <v>0</v>
-      </c>
-      <c r="X40" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="11">
-        <v>144</v>
-      </c>
-      <c r="AD40" s="11">
-        <v>4</v>
-      </c>
-      <c r="AE40" s="11">
-        <v>1</v>
-      </c>
-      <c r="AF40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AG40" s="11">
-        <v>6</v>
-      </c>
-      <c r="AH40" s="11">
-        <v>7</v>
-      </c>
-      <c r="AI40" s="11">
-        <v>4</v>
-      </c>
-      <c r="AJ40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AK40" s="11">
-        <v>2</v>
-      </c>
-      <c r="AL40" s="11">
-        <v>2</v>
-      </c>
-      <c r="AM40" s="11">
-        <v>11</v>
-      </c>
-      <c r="AN40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AO40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AP40" s="11">
-        <v>6</v>
-      </c>
-      <c r="AQ40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AR40" s="11">
-        <v>1</v>
-      </c>
-      <c r="AS40" s="11">
-        <v>5</v>
-      </c>
-      <c r="AT40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AU40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AV40" s="11">
-        <v>11</v>
-      </c>
-      <c r="AW40" s="11">
-        <v>6</v>
-      </c>
-      <c r="AX40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AY40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ40" s="11">
-        <v>4</v>
-      </c>
-      <c r="BA40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BB40" s="11">
-        <v>9</v>
-      </c>
-      <c r="BC40" s="11">
-        <v>6</v>
-      </c>
-      <c r="BD40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BE40" s="11">
-        <v>5</v>
-      </c>
-      <c r="BF40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BG40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BH40" s="11">
-        <v>4</v>
-      </c>
-      <c r="BI40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BJ40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BK40" s="11">
-        <v>7</v>
-      </c>
-      <c r="BL40" s="11">
-        <v>4</v>
-      </c>
-      <c r="BM40" s="11">
-        <v>11</v>
-      </c>
-      <c r="BN40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BO40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP40" s="12">
-        <f t="shared" si="4"/>
-        <v>287</v>
-      </c>
-    </row>
-    <row r="41" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
-        <v>39</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="8">
-        <f t="shared" si="0"/>
-        <v>80.375</v>
-      </c>
-      <c r="D41" s="9">
-        <f t="shared" si="1"/>
-        <v>228.18213280106434</v>
-      </c>
-      <c r="E41" s="9">
-        <f t="shared" si="2"/>
-        <v>764.92139840319305</v>
-      </c>
-      <c r="F41" s="10">
-        <f t="shared" si="3"/>
-        <v>-604.17139840319305</v>
-      </c>
-      <c r="G41" s="11">
-        <v>0</v>
-      </c>
-      <c r="H41" s="11">
-        <v>0</v>
-      </c>
-      <c r="I41" s="11">
-        <v>0</v>
-      </c>
-      <c r="J41" s="11">
-        <v>0</v>
-      </c>
-      <c r="K41" s="11">
-        <v>0</v>
-      </c>
-      <c r="L41" s="11">
-        <v>836</v>
-      </c>
-      <c r="M41" s="11">
-        <v>14</v>
-      </c>
-      <c r="N41" s="11">
-        <v>23</v>
-      </c>
-      <c r="O41" s="11">
-        <v>3</v>
-      </c>
-      <c r="P41" s="11">
-        <v>11</v>
-      </c>
-      <c r="Q41" s="11">
-        <v>12</v>
-      </c>
-      <c r="R41" s="11">
-        <v>10</v>
-      </c>
-      <c r="S41" s="11">
-        <v>20</v>
-      </c>
-      <c r="T41" s="11">
-        <v>27</v>
-      </c>
-      <c r="U41" s="11">
-        <v>11</v>
-      </c>
-      <c r="V41" s="11">
-        <v>26</v>
-      </c>
-      <c r="W41" s="11">
-        <v>12</v>
-      </c>
-      <c r="X41" s="11">
-        <v>132</v>
-      </c>
-      <c r="Y41" s="11">
-        <v>17</v>
-      </c>
-      <c r="Z41" s="11">
-        <v>7</v>
-      </c>
-      <c r="AA41" s="11">
-        <v>28</v>
-      </c>
-      <c r="AB41" s="11">
-        <v>22</v>
-      </c>
-      <c r="AC41" s="11">
-        <v>17</v>
-      </c>
-      <c r="AD41" s="11">
-        <v>22</v>
-      </c>
-      <c r="AE41" s="11">
-        <v>29</v>
-      </c>
-      <c r="AF41" s="11">
-        <v>32</v>
-      </c>
-      <c r="AG41" s="11">
-        <v>35</v>
-      </c>
-      <c r="AH41" s="11">
-        <v>34</v>
-      </c>
-      <c r="AI41" s="11">
-        <v>27</v>
-      </c>
-      <c r="AJ41" s="11">
-        <v>141</v>
-      </c>
-      <c r="AK41" s="11">
-        <v>18</v>
-      </c>
-      <c r="AL41" s="11">
-        <v>30</v>
-      </c>
-      <c r="AM41" s="11">
-        <v>26</v>
-      </c>
-      <c r="AN41" s="11">
-        <v>14</v>
-      </c>
-      <c r="AO41" s="11">
-        <v>27</v>
-      </c>
-      <c r="AP41" s="11">
-        <v>49</v>
-      </c>
-      <c r="AQ41" s="11">
-        <v>24</v>
-      </c>
-      <c r="AR41" s="11">
-        <v>59</v>
-      </c>
-      <c r="AS41" s="11">
-        <v>24</v>
-      </c>
-      <c r="AT41" s="11">
-        <v>17</v>
-      </c>
-      <c r="AU41" s="11">
-        <v>33</v>
-      </c>
-      <c r="AV41" s="11">
-        <v>1578</v>
-      </c>
-      <c r="AW41" s="11">
-        <v>21</v>
-      </c>
-      <c r="AX41" s="11">
-        <v>35</v>
-      </c>
-      <c r="AY41" s="11">
-        <v>19</v>
-      </c>
-      <c r="AZ41" s="11">
-        <v>23</v>
-      </c>
-      <c r="BA41" s="11">
-        <v>37</v>
-      </c>
-      <c r="BB41" s="11">
-        <v>23</v>
-      </c>
-      <c r="BC41" s="11">
-        <v>16</v>
-      </c>
-      <c r="BD41" s="11">
-        <v>38</v>
-      </c>
-      <c r="BE41" s="11">
-        <v>47</v>
-      </c>
-      <c r="BF41" s="11">
-        <v>34</v>
-      </c>
-      <c r="BG41" s="11">
-        <v>28</v>
-      </c>
-      <c r="BH41" s="11">
-        <v>73</v>
-      </c>
-      <c r="BI41" s="11">
-        <v>42</v>
-      </c>
-      <c r="BJ41" s="11">
-        <v>27</v>
-      </c>
-      <c r="BK41" s="11">
-        <v>36</v>
-      </c>
-      <c r="BL41" s="11">
-        <v>32</v>
-      </c>
-      <c r="BM41" s="11">
-        <v>20</v>
-      </c>
-      <c r="BN41" s="11">
-        <v>489</v>
-      </c>
-      <c r="BO41" s="11">
-        <v>14</v>
-      </c>
-      <c r="BP41" s="12">
-        <f t="shared" si="4"/>
-        <v>4501</v>
-      </c>
-    </row>
-    <row r="42" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="C32"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43"/>
     </row>
-    <row r="44" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
@@ -9411,53 +7091,17 @@
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="G3:BO3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+  <conditionalFormatting sqref="G3:BO29">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
       <formula>$E3</formula>
       <formula>$F3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:BO41">
+  <conditionalFormatting sqref="G30:BO30">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
-      <formula>$E4</formula>
-      <formula>$F4</formula>
+      <formula>$E30</formula>
+      <formula>$F30</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dummy data sd modified
</commit_message>
<xml_diff>
--- a/DummyDataSD.xlsx
+++ b/DummyDataSD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\dummyRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CBD8E8-4C70-44CB-BAD3-D7EE4EBB8040}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8DB9EE-BD57-48F5-AA5F-4A6D429EE7F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{53814407-132E-4781-821F-A24DB13BF6DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>sigma</t>
   </si>
@@ -310,39 +310,6 @@
   </si>
   <si>
     <t>AB128</t>
-  </si>
-  <si>
-    <t>AB129</t>
-  </si>
-  <si>
-    <t>AB130</t>
-  </si>
-  <si>
-    <t>AB131</t>
-  </si>
-  <si>
-    <t>AB132</t>
-  </si>
-  <si>
-    <t>AB133</t>
-  </si>
-  <si>
-    <t>AB134</t>
-  </si>
-  <si>
-    <t>AB135</t>
-  </si>
-  <si>
-    <t>AB136</t>
-  </si>
-  <si>
-    <t>AB137</t>
-  </si>
-  <si>
-    <t>AB138</t>
-  </si>
-  <si>
-    <t>AB139</t>
   </si>
 </sst>
 </file>
@@ -806,10 +773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C5F4D2-925C-4D20-9E11-7FE796D1FD56}">
-  <dimension ref="A1:BP101"/>
+  <dimension ref="A1:BP89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B41"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,19 +1225,19 @@
         <v>68</v>
       </c>
       <c r="C4" s="8">
-        <f t="shared" ref="C4:C41" si="0">AVERAGEIF(G4:BO4,"&lt;&gt;0")</f>
+        <f t="shared" ref="C4:C29" si="0">AVERAGEIF(G4:BO4,"&lt;&gt;0")</f>
         <v>8.5399999999999991</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D41" si="1">_xlfn.STDEV.P(G4:BO4)</f>
+        <f t="shared" ref="D4:D29" si="1">_xlfn.STDEV.P(G4:BO4)</f>
         <v>9.8029771322663866</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" ref="E4:E41" si="2">C4+$E$1*D4</f>
+        <f t="shared" ref="E4:E29" si="2">C4+$E$1*D4</f>
         <v>37.948931396799161</v>
       </c>
       <c r="F4" s="10">
-        <f t="shared" ref="F4:F41" si="3">C4-$E$1*D4</f>
+        <f t="shared" ref="F4:F29" si="3">C4-$E$1*D4</f>
         <v>-20.868931396799162</v>
       </c>
       <c r="G4" s="11">
@@ -1456,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="BP4" s="12">
-        <f t="shared" ref="BP4:BP41" si="4">SUM(G4:BO4)</f>
+        <f t="shared" ref="BP4:BP29" si="4">SUM(G4:BO4)</f>
         <v>427</v>
       </c>
     </row>
@@ -5267,19 +5235,19 @@
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
-        <v>263.33333333333331</v>
+        <v>263.11764705882354</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="1"/>
-        <v>511.90310879856457</v>
+        <v>511.96220057072793</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="2"/>
-        <v>1799.042659729027</v>
+        <v>1799.0042487710075</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="3"/>
-        <v>-1272.3759930623605</v>
+        <v>-1272.7689546533602</v>
       </c>
       <c r="G23" s="11">
         <v>0</v>
@@ -5447,7 +5415,7 @@
         <v>107</v>
       </c>
       <c r="BJ23" s="11">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="BK23" s="11">
         <v>36</v>
@@ -5459,14 +5427,14 @@
         <v>24</v>
       </c>
       <c r="BN23" s="11">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BO23" s="11">
         <v>0</v>
       </c>
       <c r="BP23" s="12">
         <f t="shared" si="4"/>
-        <v>13430</v>
+        <v>13419</v>
       </c>
     </row>
     <row r="24" spans="1:68" x14ac:dyDescent="0.25">
@@ -5478,19 +5446,19 @@
       </c>
       <c r="C24" s="8">
         <f t="shared" si="0"/>
-        <v>97.6</v>
+        <v>90.51666666666668</v>
       </c>
       <c r="D24" s="9">
         <f t="shared" si="1"/>
-        <v>200.52292293638357</v>
+        <v>200.51077427906142</v>
       </c>
       <c r="E24" s="9">
         <f t="shared" si="2"/>
-        <v>699.16876880915072</v>
+        <v>692.04898950385086</v>
       </c>
       <c r="F24" s="10">
         <f t="shared" si="3"/>
-        <v>-503.96876880915067</v>
+        <v>-511.01565617051756</v>
       </c>
       <c r="G24" s="11">
         <v>0</v>
@@ -5613,7 +5581,7 @@
         <v>10</v>
       </c>
       <c r="AU24" s="11">
-        <v>8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AV24" s="11">
         <v>0</v>
@@ -5631,7 +5599,7 @@
         <v>0</v>
       </c>
       <c r="BA24" s="11">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="BB24" s="11">
         <v>0</v>
@@ -5658,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="BJ24" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK24" s="11">
         <v>0</v>
@@ -5677,7 +5645,7 @@
       </c>
       <c r="BP24" s="12">
         <f t="shared" si="4"/>
-        <v>2440</v>
+        <v>2443.9500000000003</v>
       </c>
     </row>
     <row r="25" spans="1:68" x14ac:dyDescent="0.25">
@@ -6737,44 +6705,44 @@
     </row>
     <row r="30" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C30" s="8">
-        <f t="shared" si="0"/>
-        <v>12.794871794871796</v>
+        <f t="shared" ref="C30" si="5">AVERAGEIF(G30:BO30,"&lt;&gt;0")</f>
+        <v>8.3414634146341466</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" si="1"/>
-        <v>29.289682733798951</v>
+        <f t="shared" ref="D30" si="6">_xlfn.STDEV.P(G30:BO30)</f>
+        <v>9.7245315762691327</v>
       </c>
       <c r="E30" s="9">
-        <f t="shared" si="2"/>
-        <v>100.66391999626865</v>
+        <f t="shared" ref="E30" si="7">C30+$E$1*D30</f>
+        <v>37.515058143441543</v>
       </c>
       <c r="F30" s="10">
-        <f t="shared" si="3"/>
-        <v>-75.074176406525055</v>
+        <f t="shared" ref="F30" si="8">C30-$E$1*D30</f>
+        <v>-20.832131314173253</v>
       </c>
       <c r="G30" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L30" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="11">
         <v>0</v>
@@ -6783,97 +6751,97 @@
         <v>0</v>
       </c>
       <c r="O30" s="11">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="P30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="11">
         <v>0</v>
       </c>
       <c r="R30" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S30" s="11">
         <v>0</v>
       </c>
       <c r="T30" s="11">
-        <v>229</v>
+        <v>44</v>
       </c>
       <c r="U30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V30" s="11">
         <v>1</v>
       </c>
       <c r="W30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X30" s="11">
         <v>10</v>
       </c>
       <c r="Y30" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z30" s="11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AA30" s="11">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AB30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="11">
+        <v>13</v>
+      </c>
+      <c r="AD30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AE30" s="11">
         <v>3</v>
       </c>
-      <c r="AC30" s="11">
+      <c r="AF30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AG30" s="11">
         <v>6</v>
       </c>
-      <c r="AD30" s="11">
-        <v>3</v>
-      </c>
-      <c r="AE30" s="11">
-        <v>7</v>
-      </c>
-      <c r="AF30" s="11">
+      <c r="AH30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AI30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AJ30" s="11">
+        <v>6</v>
+      </c>
+      <c r="AK30" s="11">
+        <v>11</v>
+      </c>
+      <c r="AL30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AM30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AO30" s="11">
+        <v>9</v>
+      </c>
+      <c r="AP30" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR30" s="11">
         <v>10</v>
       </c>
-      <c r="AG30" s="11">
-        <v>3</v>
-      </c>
-      <c r="AH30" s="11">
-        <v>16</v>
-      </c>
-      <c r="AI30" s="11">
-        <v>19</v>
-      </c>
-      <c r="AJ30" s="11">
-        <v>2</v>
-      </c>
-      <c r="AK30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="11">
-        <v>16</v>
-      </c>
-      <c r="AM30" s="11">
-        <v>13</v>
-      </c>
-      <c r="AN30" s="11">
-        <v>4</v>
-      </c>
-      <c r="AO30" s="11">
-        <v>12</v>
-      </c>
-      <c r="AP30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AQ30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AR30" s="11">
-        <v>37</v>
-      </c>
       <c r="AS30" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT30" s="11">
         <v>0</v>
@@ -6882,2410 +6850,122 @@
         <v>0</v>
       </c>
       <c r="AV30" s="11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AW30" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX30" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY30" s="11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AZ30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA30" s="11">
         <v>0</v>
       </c>
       <c r="BB30" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BC30" s="11">
+        <v>0</v>
+      </c>
+      <c r="BD30" s="11">
         <v>11</v>
       </c>
-      <c r="BD30" s="11">
-        <v>20</v>
-      </c>
       <c r="BE30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF30" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BG30" s="11">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BH30" s="11">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="BI30" s="11">
         <v>0</v>
       </c>
       <c r="BJ30" s="11">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="BK30" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BL30" s="11">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="BM30" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BN30" s="11">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="BO30" s="11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="BP30" s="12">
-        <f t="shared" si="4"/>
-        <v>499</v>
+        <f t="shared" ref="BP30" si="9">SUM(G30:BO30)</f>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="8">
-        <f t="shared" si="0"/>
-        <v>217.84090909090909</v>
-      </c>
-      <c r="D31" s="9">
-        <f t="shared" si="1"/>
-        <v>542.07955605741529</v>
-      </c>
-      <c r="E31" s="9">
-        <f t="shared" si="2"/>
-        <v>1844.079577263155</v>
-      </c>
-      <c r="F31" s="10">
-        <f t="shared" si="3"/>
-        <v>-1408.397759081337</v>
-      </c>
-      <c r="G31" s="11">
-        <v>0</v>
-      </c>
-      <c r="H31" s="11">
-        <v>0</v>
-      </c>
-      <c r="I31" s="11">
-        <v>0</v>
-      </c>
-      <c r="J31" s="11">
-        <v>0</v>
-      </c>
-      <c r="K31" s="11">
-        <v>0</v>
-      </c>
-      <c r="L31" s="11">
-        <v>0</v>
-      </c>
-      <c r="M31" s="11">
-        <v>0</v>
-      </c>
-      <c r="N31" s="11">
-        <v>0</v>
-      </c>
-      <c r="O31" s="11">
-        <v>0</v>
-      </c>
-      <c r="P31" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="11">
-        <v>0</v>
-      </c>
-      <c r="R31" s="11">
-        <v>0</v>
-      </c>
-      <c r="S31" s="11">
-        <v>0</v>
-      </c>
-      <c r="T31" s="11">
-        <v>0</v>
-      </c>
-      <c r="U31" s="11">
-        <v>0</v>
-      </c>
-      <c r="V31" s="11">
-        <v>0</v>
-      </c>
-      <c r="W31" s="11">
-        <v>0</v>
-      </c>
-      <c r="X31" s="11">
-        <v>3735</v>
-      </c>
-      <c r="Y31" s="11">
-        <v>76</v>
-      </c>
-      <c r="Z31" s="11">
-        <v>58</v>
-      </c>
-      <c r="AA31" s="11">
-        <v>43</v>
-      </c>
-      <c r="AB31" s="11">
-        <v>55</v>
-      </c>
-      <c r="AC31" s="11">
-        <v>79</v>
-      </c>
-      <c r="AD31" s="11">
-        <v>64</v>
-      </c>
-      <c r="AE31" s="11">
-        <v>39</v>
-      </c>
-      <c r="AF31" s="11">
-        <v>90</v>
-      </c>
-      <c r="AG31" s="11">
-        <v>57</v>
-      </c>
-      <c r="AH31" s="11">
-        <v>61</v>
-      </c>
-      <c r="AI31" s="11">
-        <v>78</v>
-      </c>
-      <c r="AJ31" s="11">
-        <v>321</v>
-      </c>
-      <c r="AK31" s="11">
-        <v>55</v>
-      </c>
-      <c r="AL31" s="11">
-        <v>58</v>
-      </c>
-      <c r="AM31" s="11">
-        <v>59</v>
-      </c>
-      <c r="AN31" s="11">
-        <v>65</v>
-      </c>
-      <c r="AO31" s="11">
-        <v>86</v>
-      </c>
-      <c r="AP31" s="11">
-        <v>62</v>
-      </c>
-      <c r="AQ31" s="11">
-        <v>90</v>
-      </c>
-      <c r="AR31" s="11">
-        <v>52</v>
-      </c>
-      <c r="AS31" s="11">
-        <v>80</v>
-      </c>
-      <c r="AT31" s="11">
-        <v>54</v>
-      </c>
-      <c r="AU31" s="11">
-        <v>70</v>
-      </c>
-      <c r="AV31" s="11">
-        <v>958</v>
-      </c>
-      <c r="AW31" s="11">
-        <v>45</v>
-      </c>
-      <c r="AX31" s="11">
-        <v>83</v>
-      </c>
-      <c r="AY31" s="11">
-        <v>53</v>
-      </c>
-      <c r="AZ31" s="11">
-        <v>60</v>
-      </c>
-      <c r="BA31" s="11">
-        <v>49</v>
-      </c>
-      <c r="BB31" s="11">
-        <v>16</v>
-      </c>
-      <c r="BC31" s="11">
-        <v>66</v>
-      </c>
-      <c r="BD31" s="11">
-        <v>80</v>
-      </c>
-      <c r="BE31" s="11">
-        <v>78</v>
-      </c>
-      <c r="BF31" s="11">
-        <v>38</v>
-      </c>
-      <c r="BG31" s="11">
-        <v>85</v>
-      </c>
-      <c r="BH31" s="11">
-        <v>2069</v>
-      </c>
-      <c r="BI31" s="11">
-        <v>42</v>
-      </c>
-      <c r="BJ31" s="11">
-        <v>58</v>
-      </c>
-      <c r="BK31" s="11">
-        <v>50</v>
-      </c>
-      <c r="BL31" s="11">
-        <v>38</v>
-      </c>
-      <c r="BM31" s="11">
-        <v>48</v>
-      </c>
-      <c r="BN31" s="11">
-        <v>163</v>
-      </c>
-      <c r="BO31" s="11">
-        <v>19</v>
-      </c>
-      <c r="BP31" s="12">
-        <f t="shared" si="4"/>
-        <v>9585</v>
-      </c>
+      <c r="C31"/>
     </row>
     <row r="32" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="8">
-        <f t="shared" si="0"/>
-        <v>83.159090909090907</v>
-      </c>
-      <c r="D32" s="9">
-        <f t="shared" si="1"/>
-        <v>232.81340532380895</v>
-      </c>
-      <c r="E32" s="9">
-        <f t="shared" si="2"/>
-        <v>781.5993068805177</v>
-      </c>
-      <c r="F32" s="10">
-        <f t="shared" si="3"/>
-        <v>-615.28112506233595</v>
-      </c>
-      <c r="G32" s="11">
-        <v>0</v>
-      </c>
-      <c r="H32" s="11">
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
-        <v>0</v>
-      </c>
-      <c r="J32" s="11">
-        <v>0</v>
-      </c>
-      <c r="K32" s="11">
-        <v>0</v>
-      </c>
-      <c r="L32" s="11">
-        <v>0</v>
-      </c>
-      <c r="M32" s="11">
-        <v>0</v>
-      </c>
-      <c r="N32" s="11">
-        <v>0</v>
-      </c>
-      <c r="O32" s="11">
-        <v>0</v>
-      </c>
-      <c r="P32" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="11">
-        <v>0</v>
-      </c>
-      <c r="R32" s="11">
-        <v>0</v>
-      </c>
-      <c r="S32" s="11">
-        <v>0</v>
-      </c>
-      <c r="T32" s="11">
-        <v>0</v>
-      </c>
-      <c r="U32" s="11">
-        <v>0</v>
-      </c>
-      <c r="V32" s="11">
-        <v>0</v>
-      </c>
-      <c r="W32" s="11">
-        <v>0</v>
-      </c>
-      <c r="X32" s="11">
-        <v>1839</v>
-      </c>
-      <c r="Y32" s="11">
-        <v>19</v>
-      </c>
-      <c r="Z32" s="11">
-        <v>14</v>
-      </c>
-      <c r="AA32" s="11">
-        <v>11</v>
-      </c>
-      <c r="AB32" s="11">
-        <v>20</v>
-      </c>
-      <c r="AC32" s="11">
-        <v>45</v>
-      </c>
-      <c r="AD32" s="11">
-        <v>33</v>
-      </c>
-      <c r="AE32" s="11">
-        <v>27</v>
-      </c>
-      <c r="AF32" s="11">
-        <v>30</v>
-      </c>
-      <c r="AG32" s="11">
-        <v>11</v>
-      </c>
-      <c r="AH32" s="11">
-        <v>12</v>
-      </c>
-      <c r="AI32" s="11">
-        <v>32</v>
-      </c>
-      <c r="AJ32" s="11">
-        <v>211</v>
-      </c>
-      <c r="AK32" s="11">
-        <v>36</v>
-      </c>
-      <c r="AL32" s="11">
-        <v>18</v>
-      </c>
-      <c r="AM32" s="11">
-        <v>16</v>
-      </c>
-      <c r="AN32" s="11">
-        <v>29</v>
-      </c>
-      <c r="AO32" s="11">
-        <v>43</v>
-      </c>
-      <c r="AP32" s="11">
-        <v>52</v>
-      </c>
-      <c r="AQ32" s="11">
-        <v>37</v>
-      </c>
-      <c r="AR32" s="11">
-        <v>32</v>
-      </c>
-      <c r="AS32" s="11">
-        <v>76</v>
-      </c>
-      <c r="AT32" s="11">
-        <v>124</v>
-      </c>
-      <c r="AU32" s="11">
-        <v>21</v>
-      </c>
-      <c r="AV32" s="11">
-        <v>134</v>
-      </c>
-      <c r="AW32" s="11">
-        <v>22</v>
-      </c>
-      <c r="AX32" s="11">
-        <v>25</v>
-      </c>
-      <c r="AY32" s="11">
-        <v>28</v>
-      </c>
-      <c r="AZ32" s="11">
-        <v>26</v>
-      </c>
-      <c r="BA32" s="11">
-        <v>40</v>
-      </c>
-      <c r="BB32" s="11">
-        <v>54</v>
-      </c>
-      <c r="BC32" s="11">
-        <v>52</v>
-      </c>
-      <c r="BD32" s="11">
-        <v>65</v>
-      </c>
-      <c r="BE32" s="11">
-        <v>38</v>
-      </c>
-      <c r="BF32" s="11">
-        <v>34</v>
-      </c>
-      <c r="BG32" s="11">
-        <v>64</v>
-      </c>
-      <c r="BH32" s="11">
-        <v>137</v>
-      </c>
-      <c r="BI32" s="11">
-        <v>16</v>
-      </c>
-      <c r="BJ32" s="11">
-        <v>32</v>
-      </c>
-      <c r="BK32" s="11">
-        <v>25</v>
-      </c>
-      <c r="BL32" s="11">
-        <v>19</v>
-      </c>
-      <c r="BM32" s="11">
-        <v>17</v>
-      </c>
-      <c r="BN32" s="11">
-        <v>28</v>
-      </c>
-      <c r="BO32" s="11">
-        <v>15</v>
-      </c>
-      <c r="BP32" s="12">
-        <f t="shared" si="4"/>
-        <v>3659</v>
-      </c>
-    </row>
-    <row r="33" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="8">
-        <f t="shared" si="0"/>
-        <v>13.475409836065573</v>
-      </c>
-      <c r="D33" s="9">
-        <f t="shared" si="1"/>
-        <v>8.3088074095949125</v>
-      </c>
-      <c r="E33" s="9">
-        <f t="shared" si="2"/>
-        <v>38.401832064850311</v>
-      </c>
-      <c r="F33" s="10">
-        <f t="shared" si="3"/>
-        <v>-11.451012392719164</v>
-      </c>
-      <c r="G33" s="11">
-        <v>14</v>
-      </c>
-      <c r="H33" s="11">
-        <v>5</v>
-      </c>
-      <c r="I33" s="11">
-        <v>25</v>
-      </c>
-      <c r="J33" s="11">
-        <v>9</v>
-      </c>
-      <c r="K33" s="11">
-        <v>2</v>
-      </c>
-      <c r="L33" s="11">
-        <v>19</v>
-      </c>
-      <c r="M33" s="11">
-        <v>13</v>
-      </c>
-      <c r="N33" s="11">
-        <v>12</v>
-      </c>
-      <c r="O33" s="11">
-        <v>14</v>
-      </c>
-      <c r="P33" s="11">
-        <v>8</v>
-      </c>
-      <c r="Q33" s="11">
-        <v>11</v>
-      </c>
-      <c r="R33" s="11">
-        <v>15</v>
-      </c>
-      <c r="S33" s="11">
-        <v>10</v>
-      </c>
-      <c r="T33" s="11">
-        <v>12</v>
-      </c>
-      <c r="U33" s="11">
-        <v>24</v>
-      </c>
-      <c r="V33" s="11">
-        <v>16</v>
-      </c>
-      <c r="W33" s="11">
-        <v>13</v>
-      </c>
-      <c r="X33" s="11">
-        <v>18</v>
-      </c>
-      <c r="Y33" s="11">
-        <v>11</v>
-      </c>
-      <c r="Z33" s="11">
-        <v>8</v>
-      </c>
-      <c r="AA33" s="11">
-        <v>2</v>
-      </c>
-      <c r="AB33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AC33" s="11">
-        <v>17</v>
-      </c>
-      <c r="AD33" s="11">
-        <v>14</v>
-      </c>
-      <c r="AE33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AF33" s="11">
-        <v>9</v>
-      </c>
-      <c r="AG33" s="11">
-        <v>40</v>
-      </c>
-      <c r="AH33" s="11">
-        <v>12</v>
-      </c>
-      <c r="AI33" s="11">
-        <v>13</v>
-      </c>
-      <c r="AJ33" s="11">
-        <v>13</v>
-      </c>
-      <c r="AK33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AL33" s="11">
-        <v>20</v>
-      </c>
-      <c r="AM33" s="11">
-        <v>10</v>
-      </c>
-      <c r="AN33" s="11">
-        <v>8</v>
-      </c>
-      <c r="AO33" s="11">
-        <v>19</v>
-      </c>
-      <c r="AP33" s="11">
-        <v>11</v>
-      </c>
-      <c r="AQ33" s="11">
-        <v>13</v>
-      </c>
-      <c r="AR33" s="11">
-        <v>19</v>
-      </c>
-      <c r="AS33" s="11">
-        <v>6</v>
-      </c>
-      <c r="AT33" s="11">
-        <v>16</v>
-      </c>
-      <c r="AU33" s="11">
-        <v>9</v>
-      </c>
-      <c r="AV33" s="11">
-        <v>29</v>
-      </c>
-      <c r="AW33" s="11">
-        <v>15</v>
-      </c>
-      <c r="AX33" s="11">
-        <v>5</v>
-      </c>
-      <c r="AY33" s="11">
-        <v>6</v>
-      </c>
-      <c r="AZ33" s="11">
-        <v>3</v>
-      </c>
-      <c r="BA33" s="11">
-        <v>14</v>
-      </c>
-      <c r="BB33" s="11">
-        <v>17</v>
-      </c>
-      <c r="BC33" s="11">
-        <v>20</v>
-      </c>
-      <c r="BD33" s="11">
-        <v>12</v>
-      </c>
-      <c r="BE33" s="11">
-        <v>7</v>
-      </c>
-      <c r="BF33" s="11">
-        <v>9</v>
-      </c>
-      <c r="BG33" s="11">
-        <v>9</v>
-      </c>
-      <c r="BH33" s="11">
-        <v>21</v>
-      </c>
-      <c r="BI33" s="11">
-        <v>4</v>
-      </c>
-      <c r="BJ33" s="11">
-        <v>2</v>
-      </c>
-      <c r="BK33" s="11">
-        <v>21</v>
-      </c>
-      <c r="BL33" s="11">
-        <v>24</v>
-      </c>
-      <c r="BM33" s="11">
-        <v>22</v>
-      </c>
-      <c r="BN33" s="11">
-        <v>47</v>
-      </c>
-      <c r="BO33" s="11">
-        <v>10</v>
-      </c>
-      <c r="BP33" s="12">
-        <f t="shared" si="4"/>
-        <v>822</v>
-      </c>
-    </row>
-    <row r="34" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>32</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" s="8">
-        <f t="shared" si="0"/>
-        <v>18.53125</v>
-      </c>
-      <c r="D34" s="9">
-        <f t="shared" si="1"/>
-        <v>48.000044790805944</v>
-      </c>
-      <c r="E34" s="9">
-        <f t="shared" si="2"/>
-        <v>162.53138437241785</v>
-      </c>
-      <c r="F34" s="10">
-        <f t="shared" si="3"/>
-        <v>-125.46888437241785</v>
-      </c>
-      <c r="G34" s="11">
-        <v>0</v>
-      </c>
-      <c r="H34" s="11">
-        <v>0</v>
-      </c>
-      <c r="I34" s="11">
-        <v>0</v>
-      </c>
-      <c r="J34" s="11">
-        <v>0</v>
-      </c>
-      <c r="K34" s="11">
-        <v>0</v>
-      </c>
-      <c r="L34" s="11">
-        <v>0</v>
-      </c>
-      <c r="M34" s="11">
-        <v>0</v>
-      </c>
-      <c r="N34" s="11">
-        <v>0</v>
-      </c>
-      <c r="O34" s="11">
-        <v>0</v>
-      </c>
-      <c r="P34" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="11">
-        <v>0</v>
-      </c>
-      <c r="R34" s="11">
-        <v>0</v>
-      </c>
-      <c r="S34" s="11">
-        <v>0</v>
-      </c>
-      <c r="T34" s="11">
-        <v>0</v>
-      </c>
-      <c r="U34" s="11">
-        <v>0</v>
-      </c>
-      <c r="V34" s="11">
-        <v>0</v>
-      </c>
-      <c r="W34" s="11">
-        <v>0</v>
-      </c>
-      <c r="X34" s="11">
-        <v>379</v>
-      </c>
-      <c r="Y34" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="11">
-        <v>4</v>
-      </c>
-      <c r="AC34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="11">
-        <v>4</v>
-      </c>
-      <c r="AE34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="11">
-        <v>8</v>
-      </c>
-      <c r="AG34" s="11">
-        <v>6</v>
-      </c>
-      <c r="AH34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AI34" s="11">
-        <v>11</v>
-      </c>
-      <c r="AJ34" s="11">
-        <v>19</v>
-      </c>
-      <c r="AK34" s="11">
-        <v>1</v>
-      </c>
-      <c r="AL34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AM34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AN34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AO34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AP34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AQ34" s="11">
-        <v>9</v>
-      </c>
-      <c r="AR34" s="11">
-        <v>9</v>
-      </c>
-      <c r="AS34" s="11">
-        <v>22</v>
-      </c>
-      <c r="AT34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AU34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AV34" s="11">
-        <v>21</v>
-      </c>
-      <c r="AW34" s="11">
-        <v>3</v>
-      </c>
-      <c r="AX34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AY34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ34" s="11">
-        <v>2</v>
-      </c>
-      <c r="BA34" s="11">
-        <v>5</v>
-      </c>
-      <c r="BB34" s="11">
-        <v>3</v>
-      </c>
-      <c r="BC34" s="11">
-        <v>1</v>
-      </c>
-      <c r="BD34" s="11">
-        <v>8</v>
-      </c>
-      <c r="BE34" s="11">
-        <v>6</v>
-      </c>
-      <c r="BF34" s="11">
-        <v>1</v>
-      </c>
-      <c r="BG34" s="11">
-        <v>0</v>
-      </c>
-      <c r="BH34" s="11">
-        <v>20</v>
-      </c>
-      <c r="BI34" s="11">
-        <v>3</v>
-      </c>
-      <c r="BJ34" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK34" s="11">
-        <v>9</v>
-      </c>
-      <c r="BL34" s="11">
-        <v>4</v>
-      </c>
-      <c r="BM34" s="11">
-        <v>1</v>
-      </c>
-      <c r="BN34" s="11">
-        <v>11</v>
-      </c>
-      <c r="BO34" s="11">
-        <v>13</v>
-      </c>
-      <c r="BP34" s="12">
-        <f t="shared" si="4"/>
-        <v>593</v>
-      </c>
-    </row>
-    <row r="35" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>33</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="8">
-        <f t="shared" si="0"/>
-        <v>242.88888888888889</v>
-      </c>
-      <c r="D35" s="9">
-        <f t="shared" si="1"/>
-        <v>415.81600144444019</v>
-      </c>
-      <c r="E35" s="9">
-        <f t="shared" si="2"/>
-        <v>1490.3368932222095</v>
-      </c>
-      <c r="F35" s="10">
-        <f t="shared" si="3"/>
-        <v>-1004.5591154444317</v>
-      </c>
-      <c r="G35" s="11">
-        <v>0</v>
-      </c>
-      <c r="H35" s="11">
-        <v>0</v>
-      </c>
-      <c r="I35" s="11">
-        <v>0</v>
-      </c>
-      <c r="J35" s="11">
-        <v>0</v>
-      </c>
-      <c r="K35" s="11">
-        <v>0</v>
-      </c>
-      <c r="L35" s="11">
-        <v>0</v>
-      </c>
-      <c r="M35" s="11">
-        <v>0</v>
-      </c>
-      <c r="N35" s="11">
-        <v>0</v>
-      </c>
-      <c r="O35" s="11">
-        <v>0</v>
-      </c>
-      <c r="P35" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="11">
-        <v>0</v>
-      </c>
-      <c r="R35" s="11">
-        <v>0</v>
-      </c>
-      <c r="S35" s="11">
-        <v>0</v>
-      </c>
-      <c r="T35" s="11">
-        <v>0</v>
-      </c>
-      <c r="U35" s="11">
-        <v>0</v>
-      </c>
-      <c r="V35" s="11">
-        <v>0</v>
-      </c>
-      <c r="W35" s="11">
-        <v>0</v>
-      </c>
-      <c r="X35" s="11">
-        <v>1581</v>
-      </c>
-      <c r="Y35" s="11">
-        <v>29</v>
-      </c>
-      <c r="Z35" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA35" s="11">
-        <v>22</v>
-      </c>
-      <c r="AB35" s="11">
-        <v>11</v>
-      </c>
-      <c r="AC35" s="11">
-        <v>21</v>
-      </c>
-      <c r="AD35" s="11">
-        <v>48</v>
-      </c>
-      <c r="AE35" s="11">
-        <v>29</v>
-      </c>
-      <c r="AF35" s="11">
-        <v>25</v>
-      </c>
-      <c r="AG35" s="11">
-        <v>10</v>
-      </c>
-      <c r="AH35" s="11">
-        <v>23</v>
-      </c>
-      <c r="AI35" s="11">
-        <v>8</v>
-      </c>
-      <c r="AJ35" s="11">
-        <v>1680</v>
-      </c>
-      <c r="AK35" s="11">
-        <v>30</v>
-      </c>
-      <c r="AL35" s="11">
-        <v>76</v>
-      </c>
-      <c r="AM35" s="11">
-        <v>6</v>
-      </c>
-      <c r="AN35" s="11">
-        <v>35</v>
-      </c>
-      <c r="AO35" s="11">
-        <v>30</v>
-      </c>
-      <c r="AP35" s="11">
-        <v>27</v>
-      </c>
-      <c r="AQ35" s="11">
-        <v>74</v>
-      </c>
-      <c r="AR35" s="11">
-        <v>37</v>
-      </c>
-      <c r="AS35" s="11">
-        <v>30</v>
-      </c>
-      <c r="AT35" s="11">
-        <v>14</v>
-      </c>
-      <c r="AU35" s="11">
-        <v>18</v>
-      </c>
-      <c r="AV35" s="11">
-        <v>1766</v>
-      </c>
-      <c r="AW35" s="11">
-        <v>53</v>
-      </c>
-      <c r="AX35" s="11">
-        <v>22</v>
-      </c>
-      <c r="AY35" s="11">
-        <v>53</v>
-      </c>
-      <c r="AZ35" s="11">
-        <v>57</v>
-      </c>
-      <c r="BA35" s="11">
-        <v>61</v>
-      </c>
-      <c r="BB35" s="11">
-        <v>1645</v>
-      </c>
-      <c r="BC35" s="11">
-        <v>124</v>
-      </c>
-      <c r="BD35" s="11">
-        <v>107</v>
-      </c>
-      <c r="BE35" s="11">
-        <v>93</v>
-      </c>
-      <c r="BF35" s="11">
-        <v>104</v>
-      </c>
-      <c r="BG35" s="11">
-        <v>41</v>
-      </c>
-      <c r="BH35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BI35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BJ35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BL35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BM35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BN35" s="11">
-        <v>754</v>
-      </c>
-      <c r="BO35" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP35" s="12">
-        <f t="shared" si="4"/>
-        <v>8744</v>
-      </c>
-    </row>
-    <row r="36" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>34</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="8">
-        <f t="shared" si="0"/>
-        <v>471.33333333333331</v>
-      </c>
-      <c r="D36" s="9">
-        <f t="shared" si="1"/>
-        <v>919.06327322340621</v>
-      </c>
-      <c r="E36" s="9">
-        <f t="shared" si="2"/>
-        <v>3228.5231530035521</v>
-      </c>
-      <c r="F36" s="10">
-        <f t="shared" si="3"/>
-        <v>-2285.8564863368852</v>
-      </c>
-      <c r="G36" s="11">
-        <v>111</v>
-      </c>
-      <c r="H36" s="11">
-        <v>191</v>
-      </c>
-      <c r="I36" s="11">
-        <v>182</v>
-      </c>
-      <c r="J36" s="11">
-        <v>123</v>
-      </c>
-      <c r="K36" s="11">
-        <v>185</v>
-      </c>
-      <c r="L36" s="11">
-        <v>3544</v>
-      </c>
-      <c r="M36" s="11">
-        <v>148</v>
-      </c>
-      <c r="N36" s="11">
-        <v>215</v>
-      </c>
-      <c r="O36" s="11">
-        <v>124</v>
-      </c>
-      <c r="P36" s="11">
-        <v>78</v>
-      </c>
-      <c r="Q36" s="11">
-        <v>91</v>
-      </c>
-      <c r="R36" s="11">
-        <v>109</v>
-      </c>
-      <c r="S36" s="11">
-        <v>159</v>
-      </c>
-      <c r="T36" s="11">
-        <v>125</v>
-      </c>
-      <c r="U36" s="11">
-        <v>56</v>
-      </c>
-      <c r="V36" s="11">
-        <v>180</v>
-      </c>
-      <c r="W36" s="11">
-        <v>424</v>
-      </c>
-      <c r="X36" s="11">
-        <v>3030</v>
-      </c>
-      <c r="Y36" s="11">
-        <v>280</v>
-      </c>
-      <c r="Z36" s="11">
-        <v>137</v>
-      </c>
-      <c r="AA36" s="11">
-        <v>141</v>
-      </c>
-      <c r="AB36" s="11">
-        <v>143</v>
-      </c>
-      <c r="AC36" s="11">
-        <v>73</v>
-      </c>
-      <c r="AD36" s="11">
-        <v>172</v>
-      </c>
-      <c r="AE36" s="11">
-        <v>161</v>
-      </c>
-      <c r="AF36" s="11">
-        <v>206</v>
-      </c>
-      <c r="AG36" s="11">
-        <v>528</v>
-      </c>
-      <c r="AH36" s="11">
-        <v>104</v>
-      </c>
-      <c r="AI36" s="11">
-        <v>141</v>
-      </c>
-      <c r="AJ36" s="11">
-        <v>2896</v>
-      </c>
-      <c r="AK36" s="11">
-        <v>207</v>
-      </c>
-      <c r="AL36" s="11">
-        <v>69</v>
-      </c>
-      <c r="AM36" s="11">
-        <v>161</v>
-      </c>
-      <c r="AN36" s="11">
-        <v>180</v>
-      </c>
-      <c r="AO36" s="11">
-        <v>114</v>
-      </c>
-      <c r="AP36" s="11">
-        <v>124</v>
-      </c>
-      <c r="AQ36" s="11">
-        <v>118</v>
-      </c>
-      <c r="AR36" s="11">
-        <v>164</v>
-      </c>
-      <c r="AS36" s="11">
-        <v>127</v>
-      </c>
-      <c r="AT36" s="11">
-        <v>142</v>
-      </c>
-      <c r="AU36" s="11">
-        <v>106</v>
-      </c>
-      <c r="AV36" s="11">
-        <v>5015</v>
-      </c>
-      <c r="AW36" s="11">
-        <v>299</v>
-      </c>
-      <c r="AX36" s="11">
-        <v>163</v>
-      </c>
-      <c r="AY36" s="11">
-        <v>225</v>
-      </c>
-      <c r="AZ36" s="11">
-        <v>122</v>
-      </c>
-      <c r="BA36" s="11">
-        <v>428</v>
-      </c>
-      <c r="BB36" s="11">
-        <v>279</v>
-      </c>
-      <c r="BC36" s="11">
-        <v>212</v>
-      </c>
-      <c r="BD36" s="11">
-        <v>300</v>
-      </c>
-      <c r="BE36" s="11">
-        <v>278</v>
-      </c>
-      <c r="BF36" s="11">
-        <v>189</v>
-      </c>
-      <c r="BG36" s="11">
-        <v>164</v>
-      </c>
-      <c r="BH36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BI36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BJ36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BL36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BM36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BN36" s="11">
-        <v>2209</v>
-      </c>
-      <c r="BO36" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP36" s="12">
-        <f t="shared" si="4"/>
-        <v>25452</v>
-      </c>
-    </row>
-    <row r="37" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>35</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="8">
-        <f t="shared" si="0"/>
-        <v>1406</v>
-      </c>
-      <c r="D37" s="9">
-        <f t="shared" si="1"/>
-        <v>869.45953922655644</v>
-      </c>
-      <c r="E37" s="9">
-        <f t="shared" si="2"/>
-        <v>4014.3786176796693</v>
-      </c>
-      <c r="F37" s="10">
-        <f t="shared" si="3"/>
-        <v>-1202.3786176796693</v>
-      </c>
-      <c r="G37" s="11">
-        <v>0</v>
-      </c>
-      <c r="H37" s="11">
-        <v>0</v>
-      </c>
-      <c r="I37" s="11">
-        <v>0</v>
-      </c>
-      <c r="J37" s="11">
-        <v>0</v>
-      </c>
-      <c r="K37" s="11">
-        <v>0</v>
-      </c>
-      <c r="L37" s="11">
-        <v>0</v>
-      </c>
-      <c r="M37" s="11">
-        <v>0</v>
-      </c>
-      <c r="N37" s="11">
-        <v>0</v>
-      </c>
-      <c r="O37" s="11">
-        <v>0</v>
-      </c>
-      <c r="P37" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="11">
-        <v>0</v>
-      </c>
-      <c r="R37" s="11">
-        <v>0</v>
-      </c>
-      <c r="S37" s="11">
-        <v>0</v>
-      </c>
-      <c r="T37" s="11">
-        <v>0</v>
-      </c>
-      <c r="U37" s="11">
-        <v>0</v>
-      </c>
-      <c r="V37" s="11">
-        <v>0</v>
-      </c>
-      <c r="W37" s="11">
-        <v>0</v>
-      </c>
-      <c r="X37" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AG37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AJ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AK37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AM37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AN37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AO37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AP37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AQ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AR37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AS37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AT37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AU37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AV37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AW37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AX37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AY37" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BA37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BB37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BC37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BD37" s="11">
-        <v>169</v>
-      </c>
-      <c r="BE37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BF37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BG37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BH37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BI37" s="11">
-        <v>3</v>
-      </c>
-      <c r="BJ37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BK37" s="11">
-        <v>7</v>
-      </c>
-      <c r="BL37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BM37" s="11">
-        <v>3</v>
-      </c>
-      <c r="BN37" s="11">
-        <v>6848</v>
-      </c>
-      <c r="BO37" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP37" s="12">
-        <f t="shared" si="4"/>
-        <v>7030</v>
-      </c>
-    </row>
-    <row r="38" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>36</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" s="8">
-        <f t="shared" si="0"/>
-        <v>275.29090909090911</v>
-      </c>
-      <c r="D38" s="9">
-        <f t="shared" si="1"/>
-        <v>639.52708231030465</v>
-      </c>
-      <c r="E38" s="9">
-        <f t="shared" si="2"/>
-        <v>2193.8721560218232</v>
-      </c>
-      <c r="F38" s="10">
-        <f t="shared" si="3"/>
-        <v>-1643.2903378400049</v>
-      </c>
-      <c r="G38" s="11">
-        <v>0</v>
-      </c>
-      <c r="H38" s="11">
-        <v>0</v>
-      </c>
-      <c r="I38" s="11">
-        <v>0</v>
-      </c>
-      <c r="J38" s="11">
-        <v>0</v>
-      </c>
-      <c r="K38" s="11">
-        <v>0</v>
-      </c>
-      <c r="L38" s="11">
-        <v>1885</v>
-      </c>
-      <c r="M38" s="11">
-        <v>26</v>
-      </c>
-      <c r="N38" s="11">
-        <v>46</v>
-      </c>
-      <c r="O38" s="11">
-        <v>47</v>
-      </c>
-      <c r="P38" s="11">
-        <v>38</v>
-      </c>
-      <c r="Q38" s="11">
-        <v>41</v>
-      </c>
-      <c r="R38" s="11">
-        <v>60</v>
-      </c>
-      <c r="S38" s="11">
-        <v>74</v>
-      </c>
-      <c r="T38" s="11">
-        <v>40</v>
-      </c>
-      <c r="U38" s="11">
-        <v>49</v>
-      </c>
-      <c r="V38" s="11">
-        <v>75</v>
-      </c>
-      <c r="W38" s="11">
-        <v>33</v>
-      </c>
-      <c r="X38" s="11">
-        <v>2092</v>
-      </c>
-      <c r="Y38" s="11">
-        <v>36</v>
-      </c>
-      <c r="Z38" s="11">
-        <v>37</v>
-      </c>
-      <c r="AA38" s="11">
-        <v>46</v>
-      </c>
-      <c r="AB38" s="11">
-        <v>89</v>
-      </c>
-      <c r="AC38" s="11">
-        <v>35</v>
-      </c>
-      <c r="AD38" s="11">
-        <v>62</v>
-      </c>
-      <c r="AE38" s="11">
-        <v>35</v>
-      </c>
-      <c r="AF38" s="11">
-        <v>66</v>
-      </c>
-      <c r="AG38" s="11">
-        <v>39</v>
-      </c>
-      <c r="AH38" s="11">
-        <v>40</v>
-      </c>
-      <c r="AI38" s="11">
-        <v>25</v>
-      </c>
-      <c r="AJ38" s="11">
-        <v>1855</v>
-      </c>
-      <c r="AK38" s="11">
-        <v>15</v>
-      </c>
-      <c r="AL38" s="11">
-        <v>52</v>
-      </c>
-      <c r="AM38" s="11">
-        <v>49</v>
-      </c>
-      <c r="AN38" s="11">
-        <v>27</v>
-      </c>
-      <c r="AO38" s="11">
-        <v>66</v>
-      </c>
-      <c r="AP38" s="11">
-        <v>35</v>
-      </c>
-      <c r="AQ38" s="11">
-        <v>54</v>
-      </c>
-      <c r="AR38" s="11">
-        <v>37</v>
-      </c>
-      <c r="AS38" s="11">
-        <v>59</v>
-      </c>
-      <c r="AT38" s="11">
-        <v>52</v>
-      </c>
-      <c r="AU38" s="11">
-        <v>37</v>
-      </c>
-      <c r="AV38" s="11">
-        <v>2139</v>
-      </c>
-      <c r="AW38" s="11">
-        <v>41</v>
-      </c>
-      <c r="AX38" s="11">
-        <v>40</v>
-      </c>
-      <c r="AY38" s="11">
-        <v>33</v>
-      </c>
-      <c r="AZ38" s="11">
-        <v>38</v>
-      </c>
-      <c r="BA38" s="11">
-        <v>35</v>
-      </c>
-      <c r="BB38" s="11">
-        <v>39</v>
-      </c>
-      <c r="BC38" s="11">
-        <v>2995</v>
-      </c>
-      <c r="BD38" s="11">
-        <v>142</v>
-      </c>
-      <c r="BE38" s="11">
-        <v>42</v>
-      </c>
-      <c r="BF38" s="11">
-        <v>49</v>
-      </c>
-      <c r="BG38" s="11">
-        <v>14</v>
-      </c>
-      <c r="BH38" s="11">
-        <v>1914</v>
-      </c>
-      <c r="BI38" s="11">
-        <v>61</v>
-      </c>
-      <c r="BJ38" s="11">
-        <v>44</v>
-      </c>
-      <c r="BK38" s="11">
-        <v>22</v>
-      </c>
-      <c r="BL38" s="11">
-        <v>23</v>
-      </c>
-      <c r="BM38" s="11">
-        <v>23</v>
-      </c>
-      <c r="BN38" s="11">
-        <v>93</v>
-      </c>
-      <c r="BO38" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP38" s="12">
-        <f t="shared" si="4"/>
-        <v>15141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
-        <v>37</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="8">
-        <f t="shared" si="0"/>
-        <v>259.27272727272725</v>
-      </c>
-      <c r="D39" s="9">
-        <f t="shared" si="1"/>
-        <v>675.5810223931627</v>
-      </c>
-      <c r="E39" s="9">
-        <f t="shared" si="2"/>
-        <v>2286.0157944522152</v>
-      </c>
-      <c r="F39" s="10">
-        <f t="shared" si="3"/>
-        <v>-1767.470339906761</v>
-      </c>
-      <c r="G39" s="11">
-        <v>0</v>
-      </c>
-      <c r="H39" s="11">
-        <v>0</v>
-      </c>
-      <c r="I39" s="11">
-        <v>0</v>
-      </c>
-      <c r="J39" s="11">
-        <v>0</v>
-      </c>
-      <c r="K39" s="11">
-        <v>0</v>
-      </c>
-      <c r="L39" s="11">
-        <v>1856</v>
-      </c>
-      <c r="M39" s="11">
-        <v>25</v>
-      </c>
-      <c r="N39" s="11">
-        <v>15</v>
-      </c>
-      <c r="O39" s="11">
-        <v>19</v>
-      </c>
-      <c r="P39" s="11">
-        <v>30</v>
-      </c>
-      <c r="Q39" s="11">
-        <v>61</v>
-      </c>
-      <c r="R39" s="11">
-        <v>28</v>
-      </c>
-      <c r="S39" s="11">
-        <v>38</v>
-      </c>
-      <c r="T39" s="11">
-        <v>113</v>
-      </c>
-      <c r="U39" s="11">
-        <v>42</v>
-      </c>
-      <c r="V39" s="11">
-        <v>29</v>
-      </c>
-      <c r="W39" s="11">
-        <v>11</v>
-      </c>
-      <c r="X39" s="11">
-        <v>3756</v>
-      </c>
-      <c r="Y39" s="11">
-        <v>94</v>
-      </c>
-      <c r="Z39" s="11">
-        <v>41</v>
-      </c>
-      <c r="AA39" s="11">
-        <v>50</v>
-      </c>
-      <c r="AB39" s="11">
-        <v>30</v>
-      </c>
-      <c r="AC39" s="11">
-        <v>2004</v>
-      </c>
-      <c r="AD39" s="11">
-        <v>31</v>
-      </c>
-      <c r="AE39" s="11">
-        <v>85</v>
-      </c>
-      <c r="AF39" s="11">
-        <v>128</v>
-      </c>
-      <c r="AG39" s="11">
-        <v>2013</v>
-      </c>
-      <c r="AH39" s="11">
-        <v>12</v>
-      </c>
-      <c r="AI39" s="11">
-        <v>30</v>
-      </c>
-      <c r="AJ39" s="11">
-        <v>2318</v>
-      </c>
-      <c r="AK39" s="11">
-        <v>26</v>
-      </c>
-      <c r="AL39" s="11">
-        <v>14</v>
-      </c>
-      <c r="AM39" s="11">
-        <v>36</v>
-      </c>
-      <c r="AN39" s="11">
-        <v>27</v>
-      </c>
-      <c r="AO39" s="11">
-        <v>12</v>
-      </c>
-      <c r="AP39" s="11">
-        <v>44</v>
-      </c>
-      <c r="AQ39" s="11">
-        <v>21</v>
-      </c>
-      <c r="AR39" s="11">
-        <v>44</v>
-      </c>
-      <c r="AS39" s="11">
-        <v>52</v>
-      </c>
-      <c r="AT39" s="11">
-        <v>40</v>
-      </c>
-      <c r="AU39" s="11">
-        <v>99</v>
-      </c>
-      <c r="AV39" s="11">
-        <v>157</v>
-      </c>
-      <c r="AW39" s="11">
-        <v>28</v>
-      </c>
-      <c r="AX39" s="11">
-        <v>36</v>
-      </c>
-      <c r="AY39" s="11">
-        <v>19</v>
-      </c>
-      <c r="AZ39" s="11">
-        <v>29</v>
-      </c>
-      <c r="BA39" s="11">
-        <v>41</v>
-      </c>
-      <c r="BB39" s="11">
-        <v>212</v>
-      </c>
-      <c r="BC39" s="11">
-        <v>50</v>
-      </c>
-      <c r="BD39" s="11">
-        <v>44</v>
-      </c>
-      <c r="BE39" s="11">
-        <v>25</v>
-      </c>
-      <c r="BF39" s="11">
-        <v>37</v>
-      </c>
-      <c r="BG39" s="11">
-        <v>52</v>
-      </c>
-      <c r="BH39" s="11">
-        <v>57</v>
-      </c>
-      <c r="BI39" s="11">
-        <v>66</v>
-      </c>
-      <c r="BJ39" s="11">
-        <v>24</v>
-      </c>
-      <c r="BK39" s="11">
-        <v>20</v>
-      </c>
-      <c r="BL39" s="11">
-        <v>9</v>
-      </c>
-      <c r="BM39" s="11">
-        <v>19</v>
-      </c>
-      <c r="BN39" s="11">
-        <v>61</v>
-      </c>
-      <c r="BO39" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP39" s="12">
-        <f t="shared" si="4"/>
-        <v>14260</v>
-      </c>
-    </row>
-    <row r="40" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
-        <v>38</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="8">
-        <f t="shared" si="0"/>
-        <v>9.258064516129032</v>
-      </c>
-      <c r="D40" s="9">
-        <f t="shared" si="1"/>
-        <v>18.239161850076371</v>
-      </c>
-      <c r="E40" s="9">
-        <f t="shared" si="2"/>
-        <v>63.975550066358146</v>
-      </c>
-      <c r="F40" s="10">
-        <f t="shared" si="3"/>
-        <v>-45.459421034100082</v>
-      </c>
-      <c r="G40" s="11">
-        <v>0</v>
-      </c>
-      <c r="H40" s="11">
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
-        <v>0</v>
-      </c>
-      <c r="J40" s="11">
-        <v>0</v>
-      </c>
-      <c r="K40" s="11">
-        <v>0</v>
-      </c>
-      <c r="L40" s="11">
-        <v>0</v>
-      </c>
-      <c r="M40" s="11">
-        <v>0</v>
-      </c>
-      <c r="N40" s="11">
-        <v>0</v>
-      </c>
-      <c r="O40" s="11">
-        <v>0</v>
-      </c>
-      <c r="P40" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="11">
-        <v>0</v>
-      </c>
-      <c r="R40" s="11">
-        <v>0</v>
-      </c>
-      <c r="S40" s="11">
-        <v>0</v>
-      </c>
-      <c r="T40" s="11">
-        <v>0</v>
-      </c>
-      <c r="U40" s="11">
-        <v>0</v>
-      </c>
-      <c r="V40" s="11">
-        <v>0</v>
-      </c>
-      <c r="W40" s="11">
-        <v>0</v>
-      </c>
-      <c r="X40" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="11">
-        <v>144</v>
-      </c>
-      <c r="AD40" s="11">
-        <v>4</v>
-      </c>
-      <c r="AE40" s="11">
-        <v>1</v>
-      </c>
-      <c r="AF40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AG40" s="11">
-        <v>6</v>
-      </c>
-      <c r="AH40" s="11">
-        <v>7</v>
-      </c>
-      <c r="AI40" s="11">
-        <v>4</v>
-      </c>
-      <c r="AJ40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AK40" s="11">
-        <v>2</v>
-      </c>
-      <c r="AL40" s="11">
-        <v>2</v>
-      </c>
-      <c r="AM40" s="11">
-        <v>11</v>
-      </c>
-      <c r="AN40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AO40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AP40" s="11">
-        <v>6</v>
-      </c>
-      <c r="AQ40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AR40" s="11">
-        <v>1</v>
-      </c>
-      <c r="AS40" s="11">
-        <v>5</v>
-      </c>
-      <c r="AT40" s="11">
-        <v>3</v>
-      </c>
-      <c r="AU40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AV40" s="11">
-        <v>11</v>
-      </c>
-      <c r="AW40" s="11">
-        <v>6</v>
-      </c>
-      <c r="AX40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AY40" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ40" s="11">
-        <v>4</v>
-      </c>
-      <c r="BA40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BB40" s="11">
-        <v>9</v>
-      </c>
-      <c r="BC40" s="11">
-        <v>6</v>
-      </c>
-      <c r="BD40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BE40" s="11">
-        <v>5</v>
-      </c>
-      <c r="BF40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BG40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BH40" s="11">
-        <v>4</v>
-      </c>
-      <c r="BI40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BJ40" s="11">
-        <v>3</v>
-      </c>
-      <c r="BK40" s="11">
-        <v>7</v>
-      </c>
-      <c r="BL40" s="11">
-        <v>4</v>
-      </c>
-      <c r="BM40" s="11">
-        <v>11</v>
-      </c>
-      <c r="BN40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BO40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BP40" s="12">
-        <f t="shared" si="4"/>
-        <v>287</v>
-      </c>
-    </row>
-    <row r="41" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
-        <v>39</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="8">
-        <f t="shared" si="0"/>
-        <v>80.375</v>
-      </c>
-      <c r="D41" s="9">
-        <f t="shared" si="1"/>
-        <v>228.18213280106434</v>
-      </c>
-      <c r="E41" s="9">
-        <f t="shared" si="2"/>
-        <v>764.92139840319305</v>
-      </c>
-      <c r="F41" s="10">
-        <f t="shared" si="3"/>
-        <v>-604.17139840319305</v>
-      </c>
-      <c r="G41" s="11">
-        <v>0</v>
-      </c>
-      <c r="H41" s="11">
-        <v>0</v>
-      </c>
-      <c r="I41" s="11">
-        <v>0</v>
-      </c>
-      <c r="J41" s="11">
-        <v>0</v>
-      </c>
-      <c r="K41" s="11">
-        <v>0</v>
-      </c>
-      <c r="L41" s="11">
-        <v>836</v>
-      </c>
-      <c r="M41" s="11">
-        <v>14</v>
-      </c>
-      <c r="N41" s="11">
-        <v>23</v>
-      </c>
-      <c r="O41" s="11">
-        <v>3</v>
-      </c>
-      <c r="P41" s="11">
-        <v>11</v>
-      </c>
-      <c r="Q41" s="11">
-        <v>12</v>
-      </c>
-      <c r="R41" s="11">
-        <v>10</v>
-      </c>
-      <c r="S41" s="11">
-        <v>20</v>
-      </c>
-      <c r="T41" s="11">
-        <v>27</v>
-      </c>
-      <c r="U41" s="11">
-        <v>11</v>
-      </c>
-      <c r="V41" s="11">
-        <v>26</v>
-      </c>
-      <c r="W41" s="11">
-        <v>12</v>
-      </c>
-      <c r="X41" s="11">
-        <v>132</v>
-      </c>
-      <c r="Y41" s="11">
-        <v>17</v>
-      </c>
-      <c r="Z41" s="11">
-        <v>7</v>
-      </c>
-      <c r="AA41" s="11">
-        <v>28</v>
-      </c>
-      <c r="AB41" s="11">
-        <v>22</v>
-      </c>
-      <c r="AC41" s="11">
-        <v>17</v>
-      </c>
-      <c r="AD41" s="11">
-        <v>22</v>
-      </c>
-      <c r="AE41" s="11">
-        <v>29</v>
-      </c>
-      <c r="AF41" s="11">
-        <v>32</v>
-      </c>
-      <c r="AG41" s="11">
-        <v>35</v>
-      </c>
-      <c r="AH41" s="11">
-        <v>34</v>
-      </c>
-      <c r="AI41" s="11">
-        <v>27</v>
-      </c>
-      <c r="AJ41" s="11">
-        <v>141</v>
-      </c>
-      <c r="AK41" s="11">
-        <v>18</v>
-      </c>
-      <c r="AL41" s="11">
-        <v>30</v>
-      </c>
-      <c r="AM41" s="11">
-        <v>26</v>
-      </c>
-      <c r="AN41" s="11">
-        <v>14</v>
-      </c>
-      <c r="AO41" s="11">
-        <v>27</v>
-      </c>
-      <c r="AP41" s="11">
-        <v>49</v>
-      </c>
-      <c r="AQ41" s="11">
-        <v>24</v>
-      </c>
-      <c r="AR41" s="11">
-        <v>59</v>
-      </c>
-      <c r="AS41" s="11">
-        <v>24</v>
-      </c>
-      <c r="AT41" s="11">
-        <v>17</v>
-      </c>
-      <c r="AU41" s="11">
-        <v>33</v>
-      </c>
-      <c r="AV41" s="11">
-        <v>1578</v>
-      </c>
-      <c r="AW41" s="11">
-        <v>21</v>
-      </c>
-      <c r="AX41" s="11">
-        <v>35</v>
-      </c>
-      <c r="AY41" s="11">
-        <v>19</v>
-      </c>
-      <c r="AZ41" s="11">
-        <v>23</v>
-      </c>
-      <c r="BA41" s="11">
-        <v>37</v>
-      </c>
-      <c r="BB41" s="11">
-        <v>23</v>
-      </c>
-      <c r="BC41" s="11">
-        <v>16</v>
-      </c>
-      <c r="BD41" s="11">
-        <v>38</v>
-      </c>
-      <c r="BE41" s="11">
-        <v>47</v>
-      </c>
-      <c r="BF41" s="11">
-        <v>34</v>
-      </c>
-      <c r="BG41" s="11">
-        <v>28</v>
-      </c>
-      <c r="BH41" s="11">
-        <v>73</v>
-      </c>
-      <c r="BI41" s="11">
-        <v>42</v>
-      </c>
-      <c r="BJ41" s="11">
-        <v>27</v>
-      </c>
-      <c r="BK41" s="11">
-        <v>36</v>
-      </c>
-      <c r="BL41" s="11">
-        <v>32</v>
-      </c>
-      <c r="BM41" s="11">
-        <v>20</v>
-      </c>
-      <c r="BN41" s="11">
-        <v>489</v>
-      </c>
-      <c r="BO41" s="11">
-        <v>14</v>
-      </c>
-      <c r="BP41" s="12">
-        <f t="shared" si="4"/>
-        <v>4501</v>
-      </c>
-    </row>
-    <row r="42" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="C32"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43"/>
     </row>
-    <row r="44" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
@@ -9411,53 +7091,17 @@
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="G3:BO3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+  <conditionalFormatting sqref="G3:BO29">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
       <formula>$E3</formula>
       <formula>$F3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:BO41">
+  <conditionalFormatting sqref="G30:BO30">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
-      <formula>$E4</formula>
-      <formula>$F4</formula>
+      <formula>$E30</formula>
+      <formula>$F30</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>